<commit_message>
Revised TypeCheckerGeneratedTester Pass vs. Fail
</commit_message>
<xml_diff>
--- a/Quorum3/Library/Tests/TypeCheckerGenerated/Type System.xlsx
+++ b/Quorum3/Library/Tests/TypeCheckerGenerated/Type System.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="641">
   <si>
     <t>Type System</t>
   </si>
@@ -1115,156 +1115,6 @@
     <t>Fail\ImpAssignUndefinedObjectField.quorum</t>
   </si>
   <si>
-    <t>Fail\ImFailignBoolObjObject.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignBooleanObjectField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignBooleanObject.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignBooleanText.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignBooleanTextField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignIntegerNumObj.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignIntObjNumObjField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignIntObjNumber.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignIntObjObject.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignIntObjObjectField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignIntegerObject.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignIntegerObjectField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignIntegerNumber.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignIntegerNumberField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignIntegerText.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignIntegerTextField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignNumObjObject.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignNumObjObjectField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignNumObjText.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignNumObjTextField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignNumberObject.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignNumberObjectFieldField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignNumberText.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignNumberTextField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignNumberTextObj.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignNumberTextObjField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignNumberUndefined.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignNumberUndefinedField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignObjectBoolean.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignObjectBooleanField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignObjectInteger.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignObjectIntegerField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignObjectNumber.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignObjectNumberField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignObjectText.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignObjectTextField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignTextBoolean.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignTextBooleanField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignTextIntObj.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignTextIntObjField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignTextInteger.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignTextIntegerField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignTextNumObj.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignTextNumObjField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignTextNumber.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignTextNumberField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignTextObject.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignTextObjectField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignTextObjObject.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImFailignTextObjObjectField.quorum</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sub Hyper()   </t>
   </si>
   <si>
@@ -1655,21 +1505,6 @@
     <t>Fail\ExpAssignIntegerNumObjField.quorum</t>
   </si>
   <si>
-    <t>Fail\ImFailignIntegerNumObjField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImpAssignBoolObjBoolean.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImpAssignBoolObjBooleanField.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImpAssignIntObjInteger.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImpAssignIntObjIntegerField.quorum</t>
-  </si>
-  <si>
     <t>Fail\ImpAssignNumObjIntObj.quorum</t>
   </si>
   <si>
@@ -1682,24 +1517,12 @@
     <t>Fail\ImpAssignNumObjIntegerField.quorum</t>
   </si>
   <si>
-    <t>Fail\ImpAssignNumObjNumber.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImpAssignNumObjNumberField.quorum</t>
-  </si>
-  <si>
     <t>Fail\ImpAssignNumberIntObj.quorum</t>
   </si>
   <si>
     <t>Fail\ImpAssignNumberIntObjField.quorum</t>
   </si>
   <si>
-    <t>Fail\ImpAssignTextObjText.quorum</t>
-  </si>
-  <si>
-    <t>Fail\ImpAssignTextObjTextField.quorum</t>
-  </si>
-  <si>
     <t>Fail\RetAssignTextObjText.quorum</t>
   </si>
   <si>
@@ -1839,6 +1662,288 @@
   </si>
   <si>
     <t>Pass\ImpAssignTextObjObjectField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignBooleanText.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignBooleanTextField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignIntegerNumObj.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignIntObjNumObjField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignIntObjNumber.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignIntegerNumber.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignIntegerNumberField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignIntegerText.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignIntegerTextField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignNumObjText.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignNumObjTextField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignNumberText.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignNumberTextField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignNumberTextObj.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignNumberTextObjField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignNumberUndefined.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignNumberUndefinedField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignTextBoolean.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignTextBooleanField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignTextIntObj.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignTextIntObjField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignTextInteger.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignTextIntegerField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignTextNumObj.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignTextNumObjField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignTextNumber.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignTextNumberField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignBoolObjObject.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignBooleanObjectField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignBooleanObject.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignBooleanText.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignBooleanTextField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignIntegerNumObj.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignIntObjNumObjField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignIntObjNumber.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignIntObjObject.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignIntObjObjectField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignIntegerNumObjField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignIntegerNumber.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignIntegerNumberField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignIntegerObject.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignIntegerObjectField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignIntegerText.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignIntegerTextField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignNumObjObject.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignNumObjObjectField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignNumObjText.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignNumObjTextField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignNumberObject.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignNumberObjectFieldField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignNumberText.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignNumberTextField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignNumberTextObj.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignNumberTextObjField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignNumberUndefined.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignNumberUndefinedField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignObjectBoolean.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignObjectBooleanField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignObjectInteger.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignObjectIntegerField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignObjectNumber.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignObjectNumberField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignObjectText.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignObjectTextField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignTextBoolean.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignTextBooleanField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignTextIntObj.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignTextIntObjField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignTextInteger.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignTextIntegerField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignTextNumObj.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignTextNumObjField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignTextNumber.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignTextNumberField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignTextObject.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignTextObjectField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignTextObjObject.quorum</t>
+  </si>
+  <si>
+    <t>Fail\RetAssignTextObjObjectField.quorum</t>
+  </si>
+  <si>
+    <t>Pass\ImpAssignBoolObjBoolean.quorum</t>
+  </si>
+  <si>
+    <t>Pass\ImpAssignBoolObjBooleanField.quorum</t>
+  </si>
+  <si>
+    <t>Pass\ImpAssignIntObjInteger.quorum</t>
+  </si>
+  <si>
+    <t>Pass\ImpAssignIntObjIntegerField.quorum</t>
+  </si>
+  <si>
+    <t>Pass\ImpAssignNumObjNumber.quorum</t>
+  </si>
+  <si>
+    <t>Pass\ImpAssignNumObjNumberField.quorum</t>
+  </si>
+  <si>
+    <t>Pass\ImpAssignObjectBoolean.quorum</t>
+  </si>
+  <si>
+    <t>Pass\ImpAssignObjectBooleanField.quorum</t>
+  </si>
+  <si>
+    <t>Pass\ImpAssignObjectInteger.quorum</t>
+  </si>
+  <si>
+    <t>Pass\ImpAssignObjectIntegerField.quorum</t>
+  </si>
+  <si>
+    <t>Pass\ImpAssignObjectNumber.quorum</t>
+  </si>
+  <si>
+    <t>Pass\ImpAssignObjectNumberField.quorum</t>
+  </si>
+  <si>
+    <t>Pass\ImpAssignObjectText.quorum</t>
+  </si>
+  <si>
+    <t>Pass\ImpAssignObjectTextField.quorum</t>
+  </si>
+  <si>
+    <t>Pass\ImpAssignTextObjText.quorum</t>
+  </si>
+  <si>
+    <t>Pass\ImpAssignTextObjTextField.quorum</t>
   </si>
 </sst>
 </file>
@@ -2081,7 +2186,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2155,6 +2260,10 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2464,9 +2573,9 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AW114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="200" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" zoomScalePageLayoutView="200" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2516,7 +2625,7 @@
     </row>
     <row r="2" spans="1:49" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>422</v>
+        <v>372</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -2526,7 +2635,7 @@
     </row>
     <row r="4" spans="1:49" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
-        <v>423</v>
+        <v>373</v>
       </c>
       <c r="B4" s="47"/>
       <c r="C4" s="48"/>
@@ -2534,7 +2643,7 @@
       <c r="E4" s="49"/>
       <c r="F4" s="3"/>
       <c r="G4" s="46" t="s">
-        <v>531</v>
+        <v>481</v>
       </c>
       <c r="H4" s="47"/>
       <c r="I4" s="48"/>
@@ -2542,7 +2651,7 @@
       <c r="K4" s="49"/>
       <c r="L4" s="3"/>
       <c r="M4" s="46" t="s">
-        <v>530</v>
+        <v>480</v>
       </c>
       <c r="N4" s="47"/>
       <c r="O4" s="48"/>
@@ -2592,10 +2701,10 @@
         <v>105</v>
       </c>
       <c r="D5" s="44" t="s">
-        <v>532</v>
+        <v>482</v>
       </c>
       <c r="E5" s="45" t="s">
-        <v>533</v>
+        <v>483</v>
       </c>
       <c r="G5" s="42" t="str">
         <f>A5</f>
@@ -2819,10 +2928,10 @@
       <c r="I7" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="52" t="s">
         <v>258</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="K7" s="52" t="s">
         <v>259</v>
       </c>
       <c r="M7" s="15"/>
@@ -2834,10 +2943,10 @@
         <v>5</v>
       </c>
       <c r="P7" s="21" t="s">
-        <v>424</v>
+        <v>374</v>
       </c>
       <c r="Q7" s="22" t="s">
-        <v>425</v>
+        <v>375</v>
       </c>
       <c r="S7" s="15"/>
       <c r="T7" s="19" t="str">
@@ -2889,17 +2998,19 @@
       <c r="E8" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="25" t="str">
+      <c r="G8" s="54"/>
+      <c r="H8" s="19" t="str">
         <f t="shared" ref="H8:H16" si="0">$B8</f>
         <v>boolean</v>
       </c>
-      <c r="I8" s="26"/>
-      <c r="J8" s="27" t="s">
-        <v>545</v>
-      </c>
-      <c r="K8" s="28" t="s">
-        <v>546</v>
+      <c r="I8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="52" t="s">
+        <v>625</v>
+      </c>
+      <c r="K8" s="52" t="s">
+        <v>626</v>
       </c>
       <c r="M8" s="15"/>
       <c r="N8" s="25" t="str">
@@ -2908,10 +3019,10 @@
       </c>
       <c r="O8" s="26"/>
       <c r="P8" s="27" t="s">
-        <v>579</v>
+        <v>520</v>
       </c>
       <c r="Q8" s="28" t="s">
-        <v>580</v>
+        <v>521</v>
       </c>
       <c r="S8" s="15"/>
       <c r="T8" s="19" t="str">
@@ -2969,10 +3080,10 @@
         <v>IntObj</v>
       </c>
       <c r="I9" s="26"/>
-      <c r="J9" s="27" t="s">
+      <c r="J9" s="51" t="s">
         <v>260</v>
       </c>
-      <c r="K9" s="28" t="s">
+      <c r="K9" s="51" t="s">
         <v>261</v>
       </c>
       <c r="M9" s="15"/>
@@ -2982,10 +3093,10 @@
       </c>
       <c r="O9" s="26"/>
       <c r="P9" s="27" t="s">
-        <v>426</v>
+        <v>376</v>
       </c>
       <c r="Q9" s="28" t="s">
-        <v>427</v>
+        <v>377</v>
       </c>
       <c r="S9" s="15"/>
       <c r="T9" s="25" t="str">
@@ -3039,10 +3150,10 @@
         <v>integer</v>
       </c>
       <c r="I10" s="29"/>
-      <c r="J10" s="27" t="s">
+      <c r="J10" s="51" t="s">
         <v>262</v>
       </c>
-      <c r="K10" s="28" t="s">
+      <c r="K10" s="51" t="s">
         <v>263</v>
       </c>
       <c r="M10" s="15"/>
@@ -3052,10 +3163,10 @@
       </c>
       <c r="O10" s="29"/>
       <c r="P10" s="27" t="s">
-        <v>428</v>
+        <v>378</v>
       </c>
       <c r="Q10" s="28" t="s">
-        <v>429</v>
+        <v>379</v>
       </c>
       <c r="S10" s="15"/>
       <c r="T10" s="25" t="str">
@@ -3111,10 +3222,10 @@
         <v>NumObj</v>
       </c>
       <c r="I11" s="29"/>
-      <c r="J11" s="27" t="s">
+      <c r="J11" s="51" t="s">
         <v>264</v>
       </c>
-      <c r="K11" s="28" t="s">
+      <c r="K11" s="51" t="s">
         <v>265</v>
       </c>
       <c r="M11" s="15"/>
@@ -3124,10 +3235,10 @@
       </c>
       <c r="O11" s="29"/>
       <c r="P11" s="27" t="s">
-        <v>430</v>
+        <v>380</v>
       </c>
       <c r="Q11" s="28" t="s">
-        <v>431</v>
+        <v>381</v>
       </c>
       <c r="S11" s="15"/>
       <c r="T11" s="25" t="str">
@@ -3183,10 +3294,10 @@
         <v>number</v>
       </c>
       <c r="I12" s="29"/>
-      <c r="J12" s="27" t="s">
+      <c r="J12" s="51" t="s">
         <v>266</v>
       </c>
-      <c r="K12" s="28" t="s">
+      <c r="K12" s="51" t="s">
         <v>267</v>
       </c>
       <c r="M12" s="15"/>
@@ -3196,10 +3307,10 @@
       </c>
       <c r="O12" s="29"/>
       <c r="P12" s="27" t="s">
-        <v>432</v>
+        <v>382</v>
       </c>
       <c r="Q12" s="28" t="s">
-        <v>433</v>
+        <v>383</v>
       </c>
       <c r="S12" s="15"/>
       <c r="T12" s="25" t="str">
@@ -3251,9 +3362,7 @@
       <c r="E13" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G13" s="14" t="s">
-        <v>5</v>
-      </c>
+      <c r="G13" s="53"/>
       <c r="H13" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Object</v>
@@ -3261,11 +3370,11 @@
       <c r="I13" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J13" s="21" t="s">
-        <v>589</v>
-      </c>
-      <c r="K13" s="22" t="s">
-        <v>590</v>
+      <c r="J13" s="52" t="s">
+        <v>530</v>
+      </c>
+      <c r="K13" s="52" t="s">
+        <v>531</v>
       </c>
       <c r="M13" s="14"/>
       <c r="N13" s="25" t="str">
@@ -3274,10 +3383,10 @@
       </c>
       <c r="O13" s="29"/>
       <c r="P13" s="27" t="s">
-        <v>364</v>
+        <v>574</v>
       </c>
       <c r="Q13" s="28" t="s">
-        <v>365</v>
+        <v>575</v>
       </c>
       <c r="S13" s="14"/>
       <c r="T13" s="25" t="str">
@@ -3336,10 +3445,10 @@
         <v>text</v>
       </c>
       <c r="I14" s="29"/>
-      <c r="J14" s="27" t="s">
+      <c r="J14" s="51" t="s">
         <v>268</v>
       </c>
-      <c r="K14" s="28" t="s">
+      <c r="K14" s="51" t="s">
         <v>269</v>
       </c>
       <c r="M14" s="15"/>
@@ -3349,10 +3458,10 @@
       </c>
       <c r="O14" s="29"/>
       <c r="P14" s="27" t="s">
-        <v>434</v>
+        <v>384</v>
       </c>
       <c r="Q14" s="28" t="s">
-        <v>435</v>
+        <v>385</v>
       </c>
       <c r="S14" s="15"/>
       <c r="T14" s="25" t="str">
@@ -3408,10 +3517,10 @@
         <v>TextObj</v>
       </c>
       <c r="I15" s="26"/>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="51" t="s">
         <v>270</v>
       </c>
-      <c r="K15" s="28" t="s">
+      <c r="K15" s="51" t="s">
         <v>271</v>
       </c>
       <c r="M15" s="15"/>
@@ -3421,10 +3530,10 @@
       </c>
       <c r="O15" s="26"/>
       <c r="P15" s="27" t="s">
-        <v>436</v>
+        <v>386</v>
       </c>
       <c r="Q15" s="28" t="s">
-        <v>437</v>
+        <v>387</v>
       </c>
       <c r="S15" s="15"/>
       <c r="T15" s="25" t="str">
@@ -3482,10 +3591,10 @@
       <c r="I16" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J16" s="21" t="s">
+      <c r="J16" s="52" t="s">
         <v>272</v>
       </c>
-      <c r="K16" s="22" t="s">
+      <c r="K16" s="52" t="s">
         <v>273</v>
       </c>
       <c r="M16" s="15"/>
@@ -3497,10 +3606,10 @@
         <v>5</v>
       </c>
       <c r="P16" s="23" t="s">
-        <v>438</v>
+        <v>388</v>
       </c>
       <c r="Q16" s="24" t="s">
-        <v>439</v>
+        <v>389</v>
       </c>
       <c r="S16" s="15"/>
       <c r="T16" s="19" t="str">
@@ -3623,19 +3732,19 @@
       <c r="E18" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="G18" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="H18" s="25" t="str">
+      <c r="G18" s="15"/>
+      <c r="H18" s="19" t="str">
         <f>$B18</f>
         <v>BoolObj</v>
       </c>
-      <c r="I18" s="26"/>
-      <c r="J18" s="27" t="s">
-        <v>587</v>
-      </c>
-      <c r="K18" s="28" t="s">
-        <v>588</v>
+      <c r="I18" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J18" s="52" t="s">
+        <v>528</v>
+      </c>
+      <c r="K18" s="52" t="s">
+        <v>529</v>
       </c>
       <c r="M18" s="15"/>
       <c r="N18" s="25" t="str">
@@ -3644,10 +3753,10 @@
       </c>
       <c r="O18" s="26"/>
       <c r="P18" s="27" t="s">
-        <v>577</v>
+        <v>518</v>
       </c>
       <c r="Q18" s="28" t="s">
-        <v>578</v>
+        <v>519</v>
       </c>
       <c r="S18" s="15"/>
       <c r="T18" s="19" t="str">
@@ -3708,10 +3817,10 @@
       <c r="I19" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="J19" s="21" t="s">
+      <c r="J19" s="52" t="s">
         <v>274</v>
       </c>
-      <c r="K19" s="22" t="s">
+      <c r="K19" s="52" t="s">
         <v>275</v>
       </c>
       <c r="L19" s="3"/>
@@ -3724,10 +3833,10 @@
         <v>5</v>
       </c>
       <c r="P19" s="23" t="s">
-        <v>440</v>
+        <v>390</v>
       </c>
       <c r="Q19" s="24" t="s">
-        <v>441</v>
+        <v>391</v>
       </c>
       <c r="R19" s="3"/>
       <c r="S19" s="15"/>
@@ -3792,10 +3901,10 @@
         <v>IntObj</v>
       </c>
       <c r="I20" s="26"/>
-      <c r="J20" s="27" t="s">
+      <c r="J20" s="51" t="s">
         <v>276</v>
       </c>
-      <c r="K20" s="28" t="s">
+      <c r="K20" s="51" t="s">
         <v>277</v>
       </c>
       <c r="M20" s="15"/>
@@ -3805,10 +3914,10 @@
       </c>
       <c r="O20" s="26"/>
       <c r="P20" s="27" t="s">
-        <v>442</v>
+        <v>392</v>
       </c>
       <c r="Q20" s="28" t="s">
-        <v>443</v>
+        <v>393</v>
       </c>
       <c r="S20" s="15"/>
       <c r="T20" s="25" t="str">
@@ -3862,10 +3971,10 @@
         <v>integer</v>
       </c>
       <c r="I21" s="26"/>
-      <c r="J21" s="27" t="s">
+      <c r="J21" s="51" t="s">
         <v>278</v>
       </c>
-      <c r="K21" s="28" t="s">
+      <c r="K21" s="51" t="s">
         <v>279</v>
       </c>
       <c r="M21" s="15"/>
@@ -3875,10 +3984,10 @@
       </c>
       <c r="O21" s="26"/>
       <c r="P21" s="27" t="s">
-        <v>444</v>
+        <v>394</v>
       </c>
       <c r="Q21" s="28" t="s">
-        <v>445</v>
+        <v>395</v>
       </c>
       <c r="S21" s="15"/>
       <c r="T21" s="25" t="str">
@@ -3934,10 +4043,10 @@
         <v>NumObj</v>
       </c>
       <c r="I22" s="26"/>
-      <c r="J22" s="27" t="s">
+      <c r="J22" s="51" t="s">
         <v>280</v>
       </c>
-      <c r="K22" s="28" t="s">
+      <c r="K22" s="51" t="s">
         <v>281</v>
       </c>
       <c r="M22" s="15"/>
@@ -3947,10 +4056,10 @@
       </c>
       <c r="O22" s="26"/>
       <c r="P22" s="27" t="s">
-        <v>446</v>
+        <v>396</v>
       </c>
       <c r="Q22" s="28" t="s">
-        <v>447</v>
+        <v>397</v>
       </c>
       <c r="S22" s="15"/>
       <c r="T22" s="25" t="str">
@@ -4004,10 +4113,10 @@
         <v>number</v>
       </c>
       <c r="I23" s="26"/>
-      <c r="J23" s="27" t="s">
+      <c r="J23" s="51" t="s">
         <v>282</v>
       </c>
-      <c r="K23" s="28" t="s">
+      <c r="K23" s="51" t="s">
         <v>283</v>
       </c>
       <c r="M23" s="15"/>
@@ -4017,10 +4126,10 @@
       </c>
       <c r="O23" s="26"/>
       <c r="P23" s="27" t="s">
-        <v>448</v>
+        <v>398</v>
       </c>
       <c r="Q23" s="28" t="s">
-        <v>449</v>
+        <v>399</v>
       </c>
       <c r="S23" s="15"/>
       <c r="T23" s="25" t="str">
@@ -4072,9 +4181,7 @@
       <c r="E24" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G24" s="14" t="s">
-        <v>5</v>
-      </c>
+      <c r="G24" s="53"/>
       <c r="H24" s="19" t="str">
         <f t="shared" si="6"/>
         <v>Object</v>
@@ -4082,11 +4189,11 @@
       <c r="I24" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J24" s="21" t="s">
-        <v>591</v>
-      </c>
-      <c r="K24" s="22" t="s">
-        <v>590</v>
+      <c r="J24" s="52" t="s">
+        <v>532</v>
+      </c>
+      <c r="K24" s="52" t="s">
+        <v>531</v>
       </c>
       <c r="M24" s="14"/>
       <c r="N24" s="25" t="str">
@@ -4095,10 +4202,10 @@
       </c>
       <c r="O24" s="29"/>
       <c r="P24" s="27" t="s">
-        <v>366</v>
+        <v>576</v>
       </c>
       <c r="Q24" s="28" t="s">
-        <v>365</v>
+        <v>575</v>
       </c>
       <c r="S24" s="14"/>
       <c r="T24" s="25" t="str">
@@ -4159,11 +4266,11 @@
         <v>text</v>
       </c>
       <c r="I25" s="29"/>
-      <c r="J25" s="27" t="s">
-        <v>367</v>
-      </c>
-      <c r="K25" s="28" t="s">
-        <v>368</v>
+      <c r="J25" s="51" t="s">
+        <v>547</v>
+      </c>
+      <c r="K25" s="51" t="s">
+        <v>548</v>
       </c>
       <c r="M25" s="15"/>
       <c r="N25" s="25" t="str">
@@ -4172,10 +4279,10 @@
       </c>
       <c r="O25" s="29"/>
       <c r="P25" s="27" t="s">
-        <v>367</v>
+        <v>577</v>
       </c>
       <c r="Q25" s="28" t="s">
-        <v>368</v>
+        <v>578</v>
       </c>
       <c r="S25" s="15"/>
       <c r="T25" s="25" t="str">
@@ -4231,10 +4338,10 @@
         <v>TextObj</v>
       </c>
       <c r="I26" s="26"/>
-      <c r="J26" s="27" t="s">
+      <c r="J26" s="51" t="s">
         <v>284</v>
       </c>
-      <c r="K26" s="28" t="s">
+      <c r="K26" s="51" t="s">
         <v>285</v>
       </c>
       <c r="M26" s="15"/>
@@ -4244,10 +4351,10 @@
       </c>
       <c r="O26" s="26"/>
       <c r="P26" s="27" t="s">
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="Q26" s="28" t="s">
-        <v>451</v>
+        <v>401</v>
       </c>
       <c r="S26" s="15"/>
       <c r="T26" s="25" t="str">
@@ -4301,10 +4408,10 @@
         <v>undefined</v>
       </c>
       <c r="I27" s="29"/>
-      <c r="J27" s="27" t="s">
+      <c r="J27" s="51" t="s">
         <v>286</v>
       </c>
-      <c r="K27" s="28" t="s">
+      <c r="K27" s="51" t="s">
         <v>287</v>
       </c>
       <c r="M27" s="15"/>
@@ -4314,10 +4421,10 @@
       </c>
       <c r="O27" s="29"/>
       <c r="P27" s="27" t="s">
-        <v>452</v>
+        <v>402</v>
       </c>
       <c r="Q27" s="28" t="s">
-        <v>453</v>
+        <v>403</v>
       </c>
       <c r="S27" s="15"/>
       <c r="T27" s="25" t="str">
@@ -4444,10 +4551,10 @@
         <v>BoolObj</v>
       </c>
       <c r="I29" s="29"/>
-      <c r="J29" s="27" t="s">
+      <c r="J29" s="51" t="s">
         <v>288</v>
       </c>
-      <c r="K29" s="28" t="s">
+      <c r="K29" s="51" t="s">
         <v>289</v>
       </c>
       <c r="M29" s="15"/>
@@ -4457,10 +4564,10 @@
       </c>
       <c r="O29" s="29"/>
       <c r="P29" s="27" t="s">
-        <v>454</v>
+        <v>404</v>
       </c>
       <c r="Q29" s="28" t="s">
-        <v>455</v>
+        <v>405</v>
       </c>
       <c r="S29" s="15"/>
       <c r="T29" s="25" t="str">
@@ -4514,10 +4621,10 @@
         <v>boolean</v>
       </c>
       <c r="I30" s="29"/>
-      <c r="J30" s="27" t="s">
+      <c r="J30" s="51" t="s">
         <v>290</v>
       </c>
-      <c r="K30" s="28" t="s">
+      <c r="K30" s="51" t="s">
         <v>291</v>
       </c>
       <c r="M30" s="15"/>
@@ -4527,10 +4634,10 @@
       </c>
       <c r="O30" s="29"/>
       <c r="P30" s="27" t="s">
-        <v>456</v>
+        <v>406</v>
       </c>
       <c r="Q30" s="28" t="s">
-        <v>457</v>
+        <v>407</v>
       </c>
       <c r="S30" s="15"/>
       <c r="T30" s="25" t="str">
@@ -4592,10 +4699,10 @@
       <c r="I31" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="J31" s="21" t="s">
+      <c r="J31" s="52" t="s">
         <v>292</v>
       </c>
-      <c r="K31" s="22" t="s">
+      <c r="K31" s="52" t="s">
         <v>293</v>
       </c>
       <c r="M31" s="15"/>
@@ -4607,10 +4714,10 @@
         <v>5</v>
       </c>
       <c r="P31" s="23" t="s">
-        <v>458</v>
+        <v>408</v>
       </c>
       <c r="Q31" s="24" t="s">
-        <v>459</v>
+        <v>409</v>
       </c>
       <c r="S31" s="15"/>
       <c r="T31" s="19" t="str">
@@ -4663,16 +4770,18 @@
         <v>172</v>
       </c>
       <c r="G32" s="15"/>
-      <c r="H32" s="25" t="str">
+      <c r="H32" s="19" t="str">
         <f t="shared" si="12"/>
         <v>integer</v>
       </c>
-      <c r="I32" s="26"/>
-      <c r="J32" s="27" t="s">
-        <v>547</v>
-      </c>
-      <c r="K32" s="28" t="s">
-        <v>548</v>
+      <c r="I32" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J32" s="52" t="s">
+        <v>627</v>
+      </c>
+      <c r="K32" s="52" t="s">
+        <v>628</v>
       </c>
       <c r="M32" s="15"/>
       <c r="N32" s="25" t="str">
@@ -4681,10 +4790,10 @@
       </c>
       <c r="O32" s="26"/>
       <c r="P32" s="27" t="s">
-        <v>575</v>
+        <v>516</v>
       </c>
       <c r="Q32" s="28" t="s">
-        <v>576</v>
+        <v>517</v>
       </c>
       <c r="S32" s="15"/>
       <c r="T32" s="19" t="str">
@@ -4729,10 +4838,10 @@
       </c>
       <c r="C33" s="29"/>
       <c r="D33" s="27" t="s">
-        <v>539</v>
+        <v>489</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>540</v>
+        <v>490</v>
       </c>
       <c r="G33" s="15"/>
       <c r="H33" s="25" t="str">
@@ -4740,11 +4849,11 @@
         <v>NumObj</v>
       </c>
       <c r="I33" s="29"/>
-      <c r="J33" s="27" t="s">
-        <v>369</v>
-      </c>
-      <c r="K33" s="28" t="s">
-        <v>370</v>
+      <c r="J33" s="51" t="s">
+        <v>549</v>
+      </c>
+      <c r="K33" s="51" t="s">
+        <v>550</v>
       </c>
       <c r="M33" s="15"/>
       <c r="N33" s="25" t="str">
@@ -4753,10 +4862,10 @@
       </c>
       <c r="O33" s="29"/>
       <c r="P33" s="27" t="s">
-        <v>369</v>
+        <v>579</v>
       </c>
       <c r="Q33" s="28" t="s">
-        <v>370</v>
+        <v>580</v>
       </c>
       <c r="S33" s="15"/>
       <c r="T33" s="25" t="str">
@@ -4801,10 +4910,10 @@
       </c>
       <c r="C34" s="29"/>
       <c r="D34" s="27" t="s">
-        <v>541</v>
+        <v>491</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>540</v>
+        <v>490</v>
       </c>
       <c r="G34" s="15"/>
       <c r="H34" s="25" t="str">
@@ -4812,11 +4921,11 @@
         <v>number</v>
       </c>
       <c r="I34" s="29"/>
-      <c r="J34" s="27" t="s">
-        <v>371</v>
-      </c>
-      <c r="K34" s="28" t="s">
-        <v>370</v>
+      <c r="J34" s="51" t="s">
+        <v>551</v>
+      </c>
+      <c r="K34" s="51" t="s">
+        <v>550</v>
       </c>
       <c r="M34" s="15"/>
       <c r="N34" s="25" t="str">
@@ -4825,10 +4934,10 @@
       </c>
       <c r="O34" s="29"/>
       <c r="P34" s="27" t="s">
-        <v>371</v>
+        <v>581</v>
       </c>
       <c r="Q34" s="28" t="s">
-        <v>370</v>
+        <v>580</v>
       </c>
       <c r="S34" s="15"/>
       <c r="T34" s="25" t="str">
@@ -4880,9 +4989,7 @@
       <c r="E35" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="G35" s="14" t="s">
-        <v>5</v>
-      </c>
+      <c r="G35" s="14"/>
       <c r="H35" s="19" t="str">
         <f t="shared" si="12"/>
         <v>Object</v>
@@ -4890,11 +4997,11 @@
       <c r="I35" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J35" s="21" t="s">
-        <v>592</v>
-      </c>
-      <c r="K35" s="22" t="s">
-        <v>593</v>
+      <c r="J35" s="52" t="s">
+        <v>533</v>
+      </c>
+      <c r="K35" s="52" t="s">
+        <v>534</v>
       </c>
       <c r="M35" s="14"/>
       <c r="N35" s="25" t="str">
@@ -4903,10 +5010,10 @@
       </c>
       <c r="O35" s="29"/>
       <c r="P35" s="27" t="s">
-        <v>372</v>
+        <v>582</v>
       </c>
       <c r="Q35" s="28" t="s">
-        <v>373</v>
+        <v>583</v>
       </c>
       <c r="S35" s="14"/>
       <c r="T35" s="25" t="str">
@@ -4965,10 +5072,10 @@
         <v>text</v>
       </c>
       <c r="I36" s="29"/>
-      <c r="J36" s="27" t="s">
+      <c r="J36" s="51" t="s">
         <v>294</v>
       </c>
-      <c r="K36" s="28" t="s">
+      <c r="K36" s="51" t="s">
         <v>295</v>
       </c>
       <c r="M36" s="15"/>
@@ -4978,10 +5085,10 @@
       </c>
       <c r="O36" s="29"/>
       <c r="P36" s="27" t="s">
-        <v>460</v>
+        <v>410</v>
       </c>
       <c r="Q36" s="28" t="s">
-        <v>461</v>
+        <v>411</v>
       </c>
       <c r="S36" s="15"/>
       <c r="T36" s="25" t="str">
@@ -5037,10 +5144,10 @@
         <v>TextObj</v>
       </c>
       <c r="I37" s="26"/>
-      <c r="J37" s="27" t="s">
+      <c r="J37" s="51" t="s">
         <v>296</v>
       </c>
-      <c r="K37" s="28" t="s">
+      <c r="K37" s="51" t="s">
         <v>297</v>
       </c>
       <c r="M37" s="15"/>
@@ -5050,10 +5157,10 @@
       </c>
       <c r="O37" s="26"/>
       <c r="P37" s="27" t="s">
-        <v>462</v>
+        <v>412</v>
       </c>
       <c r="Q37" s="28" t="s">
-        <v>463</v>
+        <v>413</v>
       </c>
       <c r="S37" s="15"/>
       <c r="T37" s="25" t="str">
@@ -5111,10 +5218,10 @@
       <c r="I38" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J38" s="21" t="s">
+      <c r="J38" s="52" t="s">
         <v>298</v>
       </c>
-      <c r="K38" s="22" t="s">
+      <c r="K38" s="52" t="s">
         <v>299</v>
       </c>
       <c r="M38" s="15"/>
@@ -5126,10 +5233,10 @@
         <v>5</v>
       </c>
       <c r="P38" s="23" t="s">
-        <v>464</v>
+        <v>414</v>
       </c>
       <c r="Q38" s="24" t="s">
-        <v>465</v>
+        <v>415</v>
       </c>
       <c r="S38" s="15"/>
       <c r="T38" s="19" t="str">
@@ -5257,10 +5364,10 @@
         <v>BoolObj</v>
       </c>
       <c r="I40" s="29"/>
-      <c r="J40" s="27" t="s">
+      <c r="J40" s="51" t="s">
         <v>300</v>
       </c>
-      <c r="K40" s="28" t="s">
+      <c r="K40" s="51" t="s">
         <v>301</v>
       </c>
       <c r="L40" s="3"/>
@@ -5271,10 +5378,10 @@
       </c>
       <c r="O40" s="29"/>
       <c r="P40" s="27" t="s">
-        <v>466</v>
+        <v>416</v>
       </c>
       <c r="Q40" s="28" t="s">
-        <v>467</v>
+        <v>417</v>
       </c>
       <c r="R40" s="3"/>
       <c r="S40" s="15"/>
@@ -5332,10 +5439,10 @@
         <v>boolean</v>
       </c>
       <c r="I41" s="29"/>
-      <c r="J41" s="27" t="s">
+      <c r="J41" s="51" t="s">
         <v>302</v>
       </c>
-      <c r="K41" s="28" t="s">
+      <c r="K41" s="51" t="s">
         <v>303</v>
       </c>
       <c r="L41" s="3"/>
@@ -5346,10 +5453,10 @@
       </c>
       <c r="O41" s="29"/>
       <c r="P41" s="27" t="s">
-        <v>468</v>
+        <v>418</v>
       </c>
       <c r="Q41" s="28" t="s">
-        <v>469</v>
+        <v>419</v>
       </c>
       <c r="R41" s="3"/>
       <c r="S41" s="15"/>
@@ -5403,9 +5510,7 @@
         <v>185</v>
       </c>
       <c r="F42" s="3"/>
-      <c r="G42" s="15" t="s">
-        <v>5</v>
-      </c>
+      <c r="G42" s="15"/>
       <c r="H42" s="19" t="str">
         <f t="shared" si="18"/>
         <v>IntObj</v>
@@ -5413,11 +5518,11 @@
       <c r="I42" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J42" s="21" t="s">
-        <v>585</v>
-      </c>
-      <c r="K42" s="22" t="s">
-        <v>586</v>
+      <c r="J42" s="52" t="s">
+        <v>526</v>
+      </c>
+      <c r="K42" s="52" t="s">
+        <v>527</v>
       </c>
       <c r="L42" s="3"/>
       <c r="M42" s="15"/>
@@ -5427,10 +5532,10 @@
       </c>
       <c r="O42" s="26"/>
       <c r="P42" s="27" t="s">
-        <v>573</v>
+        <v>514</v>
       </c>
       <c r="Q42" s="28" t="s">
-        <v>574</v>
+        <v>515</v>
       </c>
       <c r="R42" s="3"/>
       <c r="S42" s="15"/>
@@ -5492,10 +5597,10 @@
       <c r="I43" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J43" s="21" t="s">
+      <c r="J43" s="52" t="s">
         <v>304</v>
       </c>
-      <c r="K43" s="22" t="s">
+      <c r="K43" s="52" t="s">
         <v>305</v>
       </c>
       <c r="L43" s="3"/>
@@ -5508,10 +5613,10 @@
         <v>5</v>
       </c>
       <c r="P43" s="23" t="s">
-        <v>470</v>
+        <v>420</v>
       </c>
       <c r="Q43" s="24" t="s">
-        <v>471</v>
+        <v>421</v>
       </c>
       <c r="R43" s="3"/>
       <c r="S43" s="15"/>
@@ -5565,15 +5670,13 @@
       </c>
       <c r="C44" s="29"/>
       <c r="D44" s="27" t="s">
-        <v>539</v>
+        <v>489</v>
       </c>
       <c r="E44" s="28" t="s">
-        <v>543</v>
+        <v>493</v>
       </c>
       <c r="F44" s="3"/>
-      <c r="G44" s="15" t="s">
-        <v>5</v>
-      </c>
+      <c r="G44" s="15"/>
       <c r="H44" s="19" t="str">
         <f t="shared" si="18"/>
         <v>NumObj</v>
@@ -5581,11 +5684,11 @@
       <c r="I44" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J44" s="21" t="s">
-        <v>594</v>
-      </c>
-      <c r="K44" s="22" t="s">
-        <v>595</v>
+      <c r="J44" s="52" t="s">
+        <v>535</v>
+      </c>
+      <c r="K44" s="52" t="s">
+        <v>536</v>
       </c>
       <c r="L44" s="3"/>
       <c r="M44" s="15"/>
@@ -5595,10 +5698,10 @@
       </c>
       <c r="O44" s="29"/>
       <c r="P44" s="27" t="s">
-        <v>369</v>
+        <v>579</v>
       </c>
       <c r="Q44" s="28" t="s">
-        <v>544</v>
+        <v>584</v>
       </c>
       <c r="R44" s="3"/>
       <c r="S44" s="15"/>
@@ -5658,11 +5761,11 @@
         <v>number</v>
       </c>
       <c r="I45" s="29"/>
-      <c r="J45" s="27" t="s">
-        <v>376</v>
-      </c>
-      <c r="K45" s="28" t="s">
-        <v>377</v>
+      <c r="J45" s="51" t="s">
+        <v>552</v>
+      </c>
+      <c r="K45" s="51" t="s">
+        <v>553</v>
       </c>
       <c r="L45" s="3"/>
       <c r="M45" s="15"/>
@@ -5672,10 +5775,10 @@
       </c>
       <c r="O45" s="29"/>
       <c r="P45" s="27" t="s">
-        <v>376</v>
+        <v>585</v>
       </c>
       <c r="Q45" s="28" t="s">
-        <v>377</v>
+        <v>586</v>
       </c>
       <c r="R45" s="3"/>
       <c r="S45" s="15"/>
@@ -5737,9 +5840,7 @@
         <v>157</v>
       </c>
       <c r="F46" s="3"/>
-      <c r="G46" s="14" t="s">
-        <v>5</v>
-      </c>
+      <c r="G46" s="14"/>
       <c r="H46" s="19" t="str">
         <f t="shared" si="18"/>
         <v>Object</v>
@@ -5747,11 +5848,11 @@
       <c r="I46" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J46" s="21" t="s">
-        <v>596</v>
-      </c>
-      <c r="K46" s="22" t="s">
-        <v>597</v>
+      <c r="J46" s="52" t="s">
+        <v>537</v>
+      </c>
+      <c r="K46" s="52" t="s">
+        <v>538</v>
       </c>
       <c r="L46" s="3"/>
       <c r="M46" s="14"/>
@@ -5761,10 +5862,10 @@
       </c>
       <c r="O46" s="29"/>
       <c r="P46" s="27" t="s">
-        <v>374</v>
+        <v>587</v>
       </c>
       <c r="Q46" s="28" t="s">
-        <v>375</v>
+        <v>588</v>
       </c>
       <c r="R46" s="3"/>
       <c r="S46" s="14"/>
@@ -5824,11 +5925,11 @@
         <v>text</v>
       </c>
       <c r="I47" s="29"/>
-      <c r="J47" s="27" t="s">
-        <v>378</v>
-      </c>
-      <c r="K47" s="28" t="s">
-        <v>379</v>
+      <c r="J47" s="51" t="s">
+        <v>554</v>
+      </c>
+      <c r="K47" s="51" t="s">
+        <v>555</v>
       </c>
       <c r="L47" s="3"/>
       <c r="M47" s="15"/>
@@ -5838,10 +5939,10 @@
       </c>
       <c r="O47" s="29"/>
       <c r="P47" s="27" t="s">
-        <v>378</v>
+        <v>589</v>
       </c>
       <c r="Q47" s="28" t="s">
-        <v>379</v>
+        <v>590</v>
       </c>
       <c r="R47" s="3"/>
       <c r="S47" s="15"/>
@@ -5899,10 +6000,10 @@
         <v>TextObj</v>
       </c>
       <c r="I48" s="31"/>
-      <c r="J48" s="27" t="s">
+      <c r="J48" s="51" t="s">
         <v>306</v>
       </c>
-      <c r="K48" s="28" t="s">
+      <c r="K48" s="51" t="s">
         <v>307</v>
       </c>
       <c r="L48" s="3"/>
@@ -5913,10 +6014,10 @@
       </c>
       <c r="O48" s="31"/>
       <c r="P48" s="27" t="s">
-        <v>472</v>
+        <v>422</v>
       </c>
       <c r="Q48" s="28" t="s">
-        <v>473</v>
+        <v>423</v>
       </c>
       <c r="R48" s="3"/>
       <c r="S48" s="15"/>
@@ -5974,10 +6075,10 @@
         <v>undefined</v>
       </c>
       <c r="I49" s="29"/>
-      <c r="J49" s="27" t="s">
+      <c r="J49" s="51" t="s">
         <v>308</v>
       </c>
-      <c r="K49" s="28" t="s">
+      <c r="K49" s="51" t="s">
         <v>309</v>
       </c>
       <c r="L49" s="3"/>
@@ -5988,10 +6089,10 @@
       </c>
       <c r="O49" s="29"/>
       <c r="P49" s="27" t="s">
-        <v>474</v>
+        <v>424</v>
       </c>
       <c r="Q49" s="28" t="s">
-        <v>475</v>
+        <v>425</v>
       </c>
       <c r="R49" s="3"/>
       <c r="S49" s="15"/>
@@ -6119,10 +6220,10 @@
         <v>BoolObj</v>
       </c>
       <c r="I51" s="29"/>
-      <c r="J51" s="27" t="s">
+      <c r="J51" s="51" t="s">
         <v>310</v>
       </c>
-      <c r="K51" s="28" t="s">
+      <c r="K51" s="51" t="s">
         <v>311</v>
       </c>
       <c r="M51" s="15"/>
@@ -6132,10 +6233,10 @@
       </c>
       <c r="O51" s="29"/>
       <c r="P51" s="27" t="s">
-        <v>476</v>
+        <v>426</v>
       </c>
       <c r="Q51" s="28" t="s">
-        <v>477</v>
+        <v>427</v>
       </c>
       <c r="S51" s="15"/>
       <c r="T51" s="25" t="str">
@@ -6189,10 +6290,10 @@
         <v>boolean</v>
       </c>
       <c r="I52" s="29"/>
-      <c r="J52" s="27" t="s">
+      <c r="J52" s="51" t="s">
         <v>312</v>
       </c>
-      <c r="K52" s="28" t="s">
+      <c r="K52" s="51" t="s">
         <v>313</v>
       </c>
       <c r="M52" s="15"/>
@@ -6202,10 +6303,10 @@
       </c>
       <c r="O52" s="29"/>
       <c r="P52" s="27" t="s">
-        <v>478</v>
+        <v>428</v>
       </c>
       <c r="Q52" s="28" t="s">
-        <v>479</v>
+        <v>429</v>
       </c>
       <c r="S52" s="15"/>
       <c r="T52" s="25" t="str">
@@ -6252,10 +6353,10 @@
       </c>
       <c r="C53" s="29"/>
       <c r="D53" s="27" t="s">
-        <v>542</v>
+        <v>492</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>538</v>
+        <v>488</v>
       </c>
       <c r="G53" s="15"/>
       <c r="H53" s="25" t="str">
@@ -6263,11 +6364,11 @@
         <v>IntObj</v>
       </c>
       <c r="I53" s="26"/>
-      <c r="J53" s="27" t="s">
-        <v>549</v>
-      </c>
-      <c r="K53" s="28" t="s">
-        <v>550</v>
+      <c r="J53" s="51" t="s">
+        <v>494</v>
+      </c>
+      <c r="K53" s="51" t="s">
+        <v>495</v>
       </c>
       <c r="M53" s="15"/>
       <c r="N53" s="25" t="str">
@@ -6276,10 +6377,10 @@
       </c>
       <c r="O53" s="26"/>
       <c r="P53" s="27" t="s">
-        <v>569</v>
+        <v>510</v>
       </c>
       <c r="Q53" s="28" t="s">
-        <v>570</v>
+        <v>511</v>
       </c>
       <c r="S53" s="15"/>
       <c r="T53" s="19" t="str">
@@ -6322,10 +6423,10 @@
       </c>
       <c r="C54" s="29"/>
       <c r="D54" s="27" t="s">
-        <v>534</v>
+        <v>484</v>
       </c>
       <c r="E54" s="28" t="s">
-        <v>535</v>
+        <v>485</v>
       </c>
       <c r="G54" s="15"/>
       <c r="H54" s="25" t="str">
@@ -6333,11 +6434,11 @@
         <v>integer</v>
       </c>
       <c r="I54" s="26"/>
-      <c r="J54" s="27" t="s">
-        <v>551</v>
-      </c>
-      <c r="K54" s="28" t="s">
-        <v>552</v>
+      <c r="J54" s="51" t="s">
+        <v>496</v>
+      </c>
+      <c r="K54" s="51" t="s">
+        <v>497</v>
       </c>
       <c r="M54" s="15"/>
       <c r="N54" s="25" t="str">
@@ -6346,10 +6447,10 @@
       </c>
       <c r="O54" s="26"/>
       <c r="P54" s="27" t="s">
-        <v>571</v>
+        <v>512</v>
       </c>
       <c r="Q54" s="28" t="s">
-        <v>572</v>
+        <v>513</v>
       </c>
       <c r="S54" s="15"/>
       <c r="T54" s="19" t="str">
@@ -6409,10 +6510,10 @@
       <c r="I55" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="J55" s="21" t="s">
+      <c r="J55" s="52" t="s">
         <v>314</v>
       </c>
-      <c r="K55" s="22" t="s">
+      <c r="K55" s="52" t="s">
         <v>315</v>
       </c>
       <c r="M55" s="15"/>
@@ -6424,10 +6525,10 @@
         <v>5</v>
       </c>
       <c r="P55" s="23" t="s">
-        <v>480</v>
+        <v>430</v>
       </c>
       <c r="Q55" s="24" t="s">
-        <v>481</v>
+        <v>431</v>
       </c>
       <c r="S55" s="15"/>
       <c r="T55" s="19" t="str">
@@ -6480,16 +6581,18 @@
         <v>190</v>
       </c>
       <c r="G56" s="15"/>
-      <c r="H56" s="25" t="str">
+      <c r="H56" s="19" t="str">
         <f t="shared" si="24"/>
         <v>number</v>
       </c>
-      <c r="I56" s="26"/>
-      <c r="J56" s="27" t="s">
-        <v>553</v>
-      </c>
-      <c r="K56" s="28" t="s">
-        <v>554</v>
+      <c r="I56" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J56" s="52" t="s">
+        <v>629</v>
+      </c>
+      <c r="K56" s="52" t="s">
+        <v>630</v>
       </c>
       <c r="M56" s="15"/>
       <c r="N56" s="25" t="str">
@@ -6498,10 +6601,10 @@
       </c>
       <c r="O56" s="26"/>
       <c r="P56" s="27" t="s">
-        <v>567</v>
+        <v>508</v>
       </c>
       <c r="Q56" s="28" t="s">
-        <v>568</v>
+        <v>509</v>
       </c>
       <c r="S56" s="15"/>
       <c r="T56" s="19" t="str">
@@ -6553,9 +6656,7 @@
       <c r="E57" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="G57" s="14" t="s">
-        <v>5</v>
-      </c>
+      <c r="G57" s="14"/>
       <c r="H57" s="19" t="str">
         <f t="shared" si="24"/>
         <v>Object</v>
@@ -6563,11 +6664,11 @@
       <c r="I57" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J57" s="21" t="s">
-        <v>598</v>
-      </c>
-      <c r="K57" s="22" t="s">
-        <v>599</v>
+      <c r="J57" s="52" t="s">
+        <v>539</v>
+      </c>
+      <c r="K57" s="52" t="s">
+        <v>540</v>
       </c>
       <c r="M57" s="14"/>
       <c r="N57" s="25" t="str">
@@ -6576,10 +6677,10 @@
       </c>
       <c r="O57" s="29"/>
       <c r="P57" s="27" t="s">
-        <v>380</v>
+        <v>591</v>
       </c>
       <c r="Q57" s="28" t="s">
-        <v>381</v>
+        <v>592</v>
       </c>
       <c r="S57" s="14"/>
       <c r="T57" s="25" t="str">
@@ -6638,11 +6739,11 @@
         <v>text</v>
       </c>
       <c r="I58" s="29"/>
-      <c r="J58" s="27" t="s">
-        <v>382</v>
-      </c>
-      <c r="K58" s="28" t="s">
-        <v>383</v>
+      <c r="J58" s="51" t="s">
+        <v>556</v>
+      </c>
+      <c r="K58" s="51" t="s">
+        <v>557</v>
       </c>
       <c r="M58" s="15"/>
       <c r="N58" s="25" t="str">
@@ -6651,10 +6752,10 @@
       </c>
       <c r="O58" s="29"/>
       <c r="P58" s="27" t="s">
-        <v>382</v>
+        <v>593</v>
       </c>
       <c r="Q58" s="28" t="s">
-        <v>383</v>
+        <v>594</v>
       </c>
       <c r="S58" s="15"/>
       <c r="T58" s="25" t="str">
@@ -6710,10 +6811,10 @@
         <v>TextObj</v>
       </c>
       <c r="I59" s="26"/>
-      <c r="J59" s="27" t="s">
+      <c r="J59" s="51" t="s">
         <v>316</v>
       </c>
-      <c r="K59" s="28" t="s">
+      <c r="K59" s="51" t="s">
         <v>317</v>
       </c>
       <c r="M59" s="15"/>
@@ -6723,10 +6824,10 @@
       </c>
       <c r="O59" s="26"/>
       <c r="P59" s="27" t="s">
-        <v>482</v>
+        <v>432</v>
       </c>
       <c r="Q59" s="28" t="s">
-        <v>483</v>
+        <v>433</v>
       </c>
       <c r="S59" s="15"/>
       <c r="T59" s="25" t="str">
@@ -6784,10 +6885,10 @@
       <c r="I60" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J60" s="21" t="s">
+      <c r="J60" s="52" t="s">
         <v>318</v>
       </c>
-      <c r="K60" s="22" t="s">
+      <c r="K60" s="52" t="s">
         <v>319</v>
       </c>
       <c r="M60" s="15"/>
@@ -6799,10 +6900,10 @@
         <v>5</v>
       </c>
       <c r="P60" s="23" t="s">
-        <v>484</v>
+        <v>434</v>
       </c>
       <c r="Q60" s="24" t="s">
-        <v>485</v>
+        <v>435</v>
       </c>
       <c r="S60" s="15"/>
       <c r="T60" s="19" t="str">
@@ -6929,10 +7030,10 @@
         <v>BoolObj</v>
       </c>
       <c r="I62" s="29"/>
-      <c r="J62" s="27" t="s">
+      <c r="J62" s="51" t="s">
         <v>320</v>
       </c>
-      <c r="K62" s="28" t="s">
+      <c r="K62" s="51" t="s">
         <v>321</v>
       </c>
       <c r="M62" s="15"/>
@@ -6942,10 +7043,10 @@
       </c>
       <c r="O62" s="29"/>
       <c r="P62" s="27" t="s">
-        <v>486</v>
+        <v>436</v>
       </c>
       <c r="Q62" s="28" t="s">
-        <v>487</v>
+        <v>437</v>
       </c>
       <c r="S62" s="15"/>
       <c r="T62" s="25" t="str">
@@ -6999,10 +7100,10 @@
         <v>boolean</v>
       </c>
       <c r="I63" s="29"/>
-      <c r="J63" s="27" t="s">
+      <c r="J63" s="51" t="s">
         <v>322</v>
       </c>
-      <c r="K63" s="28" t="s">
+      <c r="K63" s="51" t="s">
         <v>323</v>
       </c>
       <c r="M63" s="15"/>
@@ -7012,10 +7113,10 @@
       </c>
       <c r="O63" s="29"/>
       <c r="P63" s="27" t="s">
-        <v>488</v>
+        <v>438</v>
       </c>
       <c r="Q63" s="28" t="s">
-        <v>489</v>
+        <v>439</v>
       </c>
       <c r="S63" s="15"/>
       <c r="T63" s="25" t="str">
@@ -7062,10 +7163,10 @@
       </c>
       <c r="C64" s="26"/>
       <c r="D64" s="27" t="s">
-        <v>537</v>
+        <v>487</v>
       </c>
       <c r="E64" s="28" t="s">
-        <v>536</v>
+        <v>486</v>
       </c>
       <c r="G64" s="15"/>
       <c r="H64" s="25" t="str">
@@ -7073,11 +7174,11 @@
         <v>IntObj</v>
       </c>
       <c r="I64" s="26"/>
-      <c r="J64" s="27" t="s">
-        <v>555</v>
-      </c>
-      <c r="K64" s="28" t="s">
-        <v>556</v>
+      <c r="J64" s="51" t="s">
+        <v>498</v>
+      </c>
+      <c r="K64" s="51" t="s">
+        <v>499</v>
       </c>
       <c r="M64" s="15"/>
       <c r="N64" s="25" t="str">
@@ -7086,10 +7187,10 @@
       </c>
       <c r="O64" s="26"/>
       <c r="P64" s="27" t="s">
-        <v>565</v>
+        <v>506</v>
       </c>
       <c r="Q64" s="28" t="s">
-        <v>566</v>
+        <v>507</v>
       </c>
       <c r="S64" s="15"/>
       <c r="T64" s="19" t="str">
@@ -7147,10 +7248,10 @@
       <c r="I65" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J65" s="21" t="s">
+      <c r="J65" s="52" t="s">
         <v>324</v>
       </c>
-      <c r="K65" s="22" t="s">
+      <c r="K65" s="52" t="s">
         <v>325</v>
       </c>
       <c r="M65" s="15"/>
@@ -7162,10 +7263,10 @@
         <v>5</v>
       </c>
       <c r="P65" s="23" t="s">
-        <v>490</v>
+        <v>440</v>
       </c>
       <c r="Q65" s="24" t="s">
-        <v>491</v>
+        <v>441</v>
       </c>
       <c r="S65" s="15"/>
       <c r="T65" s="19" t="str">
@@ -7235,9 +7336,7 @@
       <c r="E66" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="G66" s="15" t="s">
-        <v>5</v>
-      </c>
+      <c r="G66" s="15"/>
       <c r="H66" s="19" t="str">
         <f t="shared" si="30"/>
         <v>NumObj</v>
@@ -7245,11 +7344,11 @@
       <c r="I66" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J66" s="21" t="s">
-        <v>583</v>
-      </c>
-      <c r="K66" s="22" t="s">
-        <v>584</v>
+      <c r="J66" s="52" t="s">
+        <v>524</v>
+      </c>
+      <c r="K66" s="52" t="s">
+        <v>525</v>
       </c>
       <c r="M66" s="15"/>
       <c r="N66" s="25" t="str">
@@ -7258,10 +7357,10 @@
       </c>
       <c r="O66" s="26"/>
       <c r="P66" s="27" t="s">
-        <v>563</v>
+        <v>504</v>
       </c>
       <c r="Q66" s="28" t="s">
-        <v>564</v>
+        <v>505</v>
       </c>
       <c r="S66" s="15"/>
       <c r="T66" s="19" t="str">
@@ -7321,10 +7420,10 @@
       <c r="I67" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="J67" s="21" t="s">
+      <c r="J67" s="52" t="s">
         <v>326</v>
       </c>
-      <c r="K67" s="22" t="s">
+      <c r="K67" s="52" t="s">
         <v>327</v>
       </c>
       <c r="M67" s="15"/>
@@ -7336,10 +7435,10 @@
         <v>5</v>
       </c>
       <c r="P67" s="23" t="s">
-        <v>492</v>
+        <v>442</v>
       </c>
       <c r="Q67" s="24" t="s">
-        <v>493</v>
+        <v>443</v>
       </c>
       <c r="S67" s="15"/>
       <c r="T67" s="19" t="str">
@@ -7409,9 +7508,7 @@
       <c r="E68" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="G68" s="14" t="s">
-        <v>5</v>
-      </c>
+      <c r="G68" s="14"/>
       <c r="H68" s="19" t="str">
         <f t="shared" si="30"/>
         <v>Object</v>
@@ -7419,11 +7516,11 @@
       <c r="I68" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J68" s="21" t="s">
-        <v>600</v>
-      </c>
-      <c r="K68" s="22" t="s">
-        <v>601</v>
+      <c r="J68" s="52" t="s">
+        <v>541</v>
+      </c>
+      <c r="K68" s="52" t="s">
+        <v>542</v>
       </c>
       <c r="M68" s="14"/>
       <c r="N68" s="25" t="str">
@@ -7432,10 +7529,10 @@
       </c>
       <c r="O68" s="29"/>
       <c r="P68" s="27" t="s">
-        <v>384</v>
+        <v>595</v>
       </c>
       <c r="Q68" s="28" t="s">
-        <v>385</v>
+        <v>596</v>
       </c>
       <c r="S68" s="14"/>
       <c r="T68" s="25" t="str">
@@ -7496,11 +7593,11 @@
         <v>text</v>
       </c>
       <c r="I69" s="29"/>
-      <c r="J69" s="27" t="s">
-        <v>386</v>
-      </c>
-      <c r="K69" s="28" t="s">
-        <v>387</v>
+      <c r="J69" s="51" t="s">
+        <v>558</v>
+      </c>
+      <c r="K69" s="51" t="s">
+        <v>559</v>
       </c>
       <c r="M69" s="15"/>
       <c r="N69" s="25" t="str">
@@ -7509,10 +7606,10 @@
       </c>
       <c r="O69" s="29"/>
       <c r="P69" s="27" t="s">
-        <v>386</v>
+        <v>597</v>
       </c>
       <c r="Q69" s="28" t="s">
-        <v>387</v>
+        <v>598</v>
       </c>
       <c r="S69" s="15"/>
       <c r="T69" s="25" t="str">
@@ -7568,11 +7665,11 @@
         <v>TextObj</v>
       </c>
       <c r="I70" s="26"/>
-      <c r="J70" s="27" t="s">
-        <v>388</v>
-      </c>
-      <c r="K70" s="28" t="s">
-        <v>389</v>
+      <c r="J70" s="51" t="s">
+        <v>560</v>
+      </c>
+      <c r="K70" s="51" t="s">
+        <v>561</v>
       </c>
       <c r="M70" s="15"/>
       <c r="N70" s="25" t="str">
@@ -7581,10 +7678,10 @@
       </c>
       <c r="O70" s="26"/>
       <c r="P70" s="27" t="s">
-        <v>388</v>
+        <v>599</v>
       </c>
       <c r="Q70" s="28" t="s">
-        <v>389</v>
+        <v>600</v>
       </c>
       <c r="S70" s="15"/>
       <c r="T70" s="25" t="str">
@@ -7638,11 +7735,11 @@
         <v>undefined</v>
       </c>
       <c r="I71" s="29"/>
-      <c r="J71" s="27" t="s">
-        <v>390</v>
-      </c>
-      <c r="K71" s="28" t="s">
-        <v>391</v>
+      <c r="J71" s="51" t="s">
+        <v>562</v>
+      </c>
+      <c r="K71" s="51" t="s">
+        <v>563</v>
       </c>
       <c r="M71" s="15"/>
       <c r="N71" s="25" t="str">
@@ -7651,10 +7748,10 @@
       </c>
       <c r="O71" s="29"/>
       <c r="P71" s="27" t="s">
-        <v>390</v>
+        <v>601</v>
       </c>
       <c r="Q71" s="28" t="s">
-        <v>391</v>
+        <v>602</v>
       </c>
       <c r="S71" s="15"/>
       <c r="T71" s="25" t="str">
@@ -7785,10 +7882,10 @@
       <c r="I73" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J73" s="21" t="s">
+      <c r="J73" s="52" t="s">
         <v>328</v>
       </c>
-      <c r="K73" s="22" t="s">
+      <c r="K73" s="52" t="s">
         <v>329</v>
       </c>
       <c r="M73" s="15"/>
@@ -7800,10 +7897,10 @@
         <v>5</v>
       </c>
       <c r="P73" s="23" t="s">
-        <v>494</v>
+        <v>444</v>
       </c>
       <c r="Q73" s="24" t="s">
-        <v>495</v>
+        <v>445</v>
       </c>
       <c r="S73" s="15"/>
       <c r="T73" s="19" t="str">
@@ -7854,16 +7951,18 @@
         <v>201</v>
       </c>
       <c r="G74" s="15"/>
-      <c r="H74" s="25" t="str">
+      <c r="H74" s="19" t="str">
         <f t="shared" ref="H74:H82" si="36">$B74</f>
         <v>boolean</v>
       </c>
-      <c r="I74" s="29"/>
-      <c r="J74" s="27" t="s">
-        <v>392</v>
-      </c>
-      <c r="K74" s="28" t="s">
-        <v>393</v>
+      <c r="I74" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J74" s="52" t="s">
+        <v>631</v>
+      </c>
+      <c r="K74" s="52" t="s">
+        <v>632</v>
       </c>
       <c r="M74" s="15"/>
       <c r="N74" s="25" t="str">
@@ -7872,10 +7971,10 @@
       </c>
       <c r="O74" s="29"/>
       <c r="P74" s="27" t="s">
-        <v>392</v>
+        <v>603</v>
       </c>
       <c r="Q74" s="28" t="s">
-        <v>393</v>
+        <v>604</v>
       </c>
       <c r="S74" s="15"/>
       <c r="T74" s="25" t="str">
@@ -7937,10 +8036,10 @@
       <c r="I75" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J75" s="21" t="s">
+      <c r="J75" s="52" t="s">
         <v>330</v>
       </c>
-      <c r="K75" s="22" t="s">
+      <c r="K75" s="52" t="s">
         <v>331</v>
       </c>
       <c r="M75" s="15"/>
@@ -7952,10 +8051,10 @@
         <v>5</v>
       </c>
       <c r="P75" s="23" t="s">
-        <v>496</v>
+        <v>446</v>
       </c>
       <c r="Q75" s="24" t="s">
-        <v>497</v>
+        <v>447</v>
       </c>
       <c r="S75" s="15"/>
       <c r="T75" s="19" t="str">
@@ -8006,16 +8105,18 @@
         <v>203</v>
       </c>
       <c r="G76" s="15"/>
-      <c r="H76" s="25" t="str">
+      <c r="H76" s="19" t="str">
         <f t="shared" si="36"/>
         <v>integer</v>
       </c>
-      <c r="I76" s="29"/>
-      <c r="J76" s="27" t="s">
-        <v>394</v>
-      </c>
-      <c r="K76" s="28" t="s">
-        <v>395</v>
+      <c r="I76" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J76" s="52" t="s">
+        <v>633</v>
+      </c>
+      <c r="K76" s="52" t="s">
+        <v>634</v>
       </c>
       <c r="M76" s="15"/>
       <c r="N76" s="25" t="str">
@@ -8024,10 +8125,10 @@
       </c>
       <c r="O76" s="29"/>
       <c r="P76" s="27" t="s">
-        <v>394</v>
+        <v>605</v>
       </c>
       <c r="Q76" s="28" t="s">
-        <v>395</v>
+        <v>606</v>
       </c>
       <c r="S76" s="15"/>
       <c r="T76" s="25" t="str">
@@ -8087,10 +8188,10 @@
       <c r="I77" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J77" s="21" t="s">
+      <c r="J77" s="52" t="s">
         <v>332</v>
       </c>
-      <c r="K77" s="22" t="s">
+      <c r="K77" s="52" t="s">
         <v>333</v>
       </c>
       <c r="M77" s="15"/>
@@ -8102,10 +8203,10 @@
         <v>5</v>
       </c>
       <c r="P77" s="23" t="s">
-        <v>498</v>
+        <v>448</v>
       </c>
       <c r="Q77" s="24" t="s">
-        <v>499</v>
+        <v>449</v>
       </c>
       <c r="S77" s="15"/>
       <c r="T77" s="19" t="str">
@@ -8156,16 +8257,18 @@
         <v>205</v>
       </c>
       <c r="G78" s="15"/>
-      <c r="H78" s="25" t="str">
+      <c r="H78" s="19" t="str">
         <f t="shared" si="36"/>
         <v>number</v>
       </c>
-      <c r="I78" s="29"/>
-      <c r="J78" s="27" t="s">
-        <v>396</v>
-      </c>
-      <c r="K78" s="28" t="s">
-        <v>397</v>
+      <c r="I78" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J78" s="52" t="s">
+        <v>635</v>
+      </c>
+      <c r="K78" s="52" t="s">
+        <v>636</v>
       </c>
       <c r="M78" s="15"/>
       <c r="N78" s="25" t="str">
@@ -8174,10 +8277,10 @@
       </c>
       <c r="O78" s="29"/>
       <c r="P78" s="27" t="s">
-        <v>396</v>
+        <v>607</v>
       </c>
       <c r="Q78" s="28" t="s">
-        <v>397</v>
+        <v>608</v>
       </c>
       <c r="S78" s="15"/>
       <c r="T78" s="25" t="str">
@@ -8237,10 +8340,10 @@
       <c r="I79" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J79" s="21" t="s">
+      <c r="J79" s="52" t="s">
         <v>334</v>
       </c>
-      <c r="K79" s="22" t="s">
+      <c r="K79" s="52" t="s">
         <v>335</v>
       </c>
       <c r="M79" s="14"/>
@@ -8252,10 +8355,10 @@
         <v>5</v>
       </c>
       <c r="P79" s="23" t="s">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="Q79" s="24" t="s">
-        <v>501</v>
+        <v>451</v>
       </c>
       <c r="S79" s="14"/>
       <c r="T79" s="19" t="str">
@@ -8308,16 +8411,18 @@
         <v>206</v>
       </c>
       <c r="G80" s="15"/>
-      <c r="H80" s="25" t="str">
+      <c r="H80" s="19" t="str">
         <f t="shared" si="36"/>
         <v>text</v>
       </c>
-      <c r="I80" s="29"/>
-      <c r="J80" s="27" t="s">
-        <v>398</v>
-      </c>
-      <c r="K80" s="28" t="s">
-        <v>399</v>
+      <c r="I80" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J80" s="52" t="s">
+        <v>637</v>
+      </c>
+      <c r="K80" s="52" t="s">
+        <v>638</v>
       </c>
       <c r="M80" s="15"/>
       <c r="N80" s="25" t="str">
@@ -8326,10 +8431,10 @@
       </c>
       <c r="O80" s="29"/>
       <c r="P80" s="27" t="s">
-        <v>398</v>
+        <v>609</v>
       </c>
       <c r="Q80" s="28" t="s">
-        <v>399</v>
+        <v>610</v>
       </c>
       <c r="S80" s="15"/>
       <c r="T80" s="25" t="str">
@@ -8407,10 +8512,10 @@
       <c r="I81" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J81" s="21" t="s">
+      <c r="J81" s="52" t="s">
         <v>336</v>
       </c>
-      <c r="K81" s="22" t="s">
+      <c r="K81" s="52" t="s">
         <v>337</v>
       </c>
       <c r="M81" s="15"/>
@@ -8422,10 +8527,10 @@
         <v>5</v>
       </c>
       <c r="P81" s="23" t="s">
-        <v>502</v>
+        <v>452</v>
       </c>
       <c r="Q81" s="24" t="s">
-        <v>503</v>
+        <v>453</v>
       </c>
       <c r="S81" s="15"/>
       <c r="T81" s="19" t="str">
@@ -8485,10 +8590,10 @@
       <c r="I82" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J82" s="21" t="s">
+      <c r="J82" s="52" t="s">
         <v>338</v>
       </c>
-      <c r="K82" s="22" t="s">
+      <c r="K82" s="52" t="s">
         <v>339</v>
       </c>
       <c r="M82" s="15"/>
@@ -8500,10 +8605,10 @@
         <v>5</v>
       </c>
       <c r="P82" s="23" t="s">
-        <v>504</v>
+        <v>454</v>
       </c>
       <c r="Q82" s="24" t="s">
-        <v>505</v>
+        <v>455</v>
       </c>
       <c r="S82" s="15"/>
       <c r="T82" s="19" t="str">
@@ -8648,10 +8753,10 @@
         <v>BoolObj</v>
       </c>
       <c r="I84" s="29"/>
-      <c r="J84" s="27" t="s">
+      <c r="J84" s="51" t="s">
         <v>340</v>
       </c>
-      <c r="K84" s="28" t="s">
+      <c r="K84" s="51" t="s">
         <v>341</v>
       </c>
       <c r="M84" s="15"/>
@@ -8661,10 +8766,10 @@
       </c>
       <c r="O84" s="29"/>
       <c r="P84" s="27" t="s">
-        <v>506</v>
+        <v>456</v>
       </c>
       <c r="Q84" s="28" t="s">
-        <v>507</v>
+        <v>457</v>
       </c>
       <c r="S84" s="15"/>
       <c r="T84" s="25" t="str">
@@ -8720,11 +8825,11 @@
         <v>boolean</v>
       </c>
       <c r="I85" s="29"/>
-      <c r="J85" s="27" t="s">
-        <v>400</v>
-      </c>
-      <c r="K85" s="28" t="s">
-        <v>401</v>
+      <c r="J85" s="51" t="s">
+        <v>564</v>
+      </c>
+      <c r="K85" s="51" t="s">
+        <v>565</v>
       </c>
       <c r="M85" s="15"/>
       <c r="N85" s="25" t="str">
@@ -8733,10 +8838,10 @@
       </c>
       <c r="O85" s="29"/>
       <c r="P85" s="27" t="s">
-        <v>400</v>
+        <v>611</v>
       </c>
       <c r="Q85" s="28" t="s">
-        <v>401</v>
+        <v>612</v>
       </c>
       <c r="S85" s="15"/>
       <c r="T85" s="25" t="str">
@@ -8794,11 +8899,11 @@
         <v>IntObj</v>
       </c>
       <c r="I86" s="29"/>
-      <c r="J86" s="27" t="s">
-        <v>402</v>
-      </c>
-      <c r="K86" s="28" t="s">
-        <v>403</v>
+      <c r="J86" s="51" t="s">
+        <v>566</v>
+      </c>
+      <c r="K86" s="51" t="s">
+        <v>567</v>
       </c>
       <c r="M86" s="15"/>
       <c r="N86" s="25" t="str">
@@ -8807,10 +8912,10 @@
       </c>
       <c r="O86" s="29"/>
       <c r="P86" s="27" t="s">
-        <v>402</v>
+        <v>613</v>
       </c>
       <c r="Q86" s="28" t="s">
-        <v>403</v>
+        <v>614</v>
       </c>
       <c r="S86" s="15"/>
       <c r="T86" s="25" t="str">
@@ -8866,11 +8971,11 @@
         <v>integer</v>
       </c>
       <c r="I87" s="29"/>
-      <c r="J87" s="27" t="s">
-        <v>404</v>
-      </c>
-      <c r="K87" s="28" t="s">
-        <v>405</v>
+      <c r="J87" s="51" t="s">
+        <v>568</v>
+      </c>
+      <c r="K87" s="51" t="s">
+        <v>569</v>
       </c>
       <c r="M87" s="15"/>
       <c r="N87" s="25" t="str">
@@ -8879,10 +8984,10 @@
       </c>
       <c r="O87" s="29"/>
       <c r="P87" s="27" t="s">
-        <v>404</v>
+        <v>615</v>
       </c>
       <c r="Q87" s="28" t="s">
-        <v>405</v>
+        <v>616</v>
       </c>
       <c r="S87" s="15"/>
       <c r="T87" s="25" t="str">
@@ -8938,11 +9043,11 @@
         <v>NumObj</v>
       </c>
       <c r="I88" s="26"/>
-      <c r="J88" s="27" t="s">
-        <v>406</v>
-      </c>
-      <c r="K88" s="28" t="s">
-        <v>407</v>
+      <c r="J88" s="51" t="s">
+        <v>570</v>
+      </c>
+      <c r="K88" s="51" t="s">
+        <v>571</v>
       </c>
       <c r="M88" s="15"/>
       <c r="N88" s="25" t="str">
@@ -8951,10 +9056,10 @@
       </c>
       <c r="O88" s="26"/>
       <c r="P88" s="27" t="s">
-        <v>406</v>
+        <v>617</v>
       </c>
       <c r="Q88" s="28" t="s">
-        <v>407</v>
+        <v>618</v>
       </c>
       <c r="S88" s="15"/>
       <c r="T88" s="25" t="str">
@@ -9010,11 +9115,11 @@
         <v>number</v>
       </c>
       <c r="I89" s="29"/>
-      <c r="J89" s="27" t="s">
-        <v>408</v>
-      </c>
-      <c r="K89" s="28" t="s">
-        <v>409</v>
+      <c r="J89" s="51" t="s">
+        <v>572</v>
+      </c>
+      <c r="K89" s="51" t="s">
+        <v>573</v>
       </c>
       <c r="M89" s="15"/>
       <c r="N89" s="25" t="str">
@@ -9023,10 +9128,10 @@
       </c>
       <c r="O89" s="29"/>
       <c r="P89" s="27" t="s">
-        <v>408</v>
+        <v>619</v>
       </c>
       <c r="Q89" s="28" t="s">
-        <v>409</v>
+        <v>620</v>
       </c>
       <c r="S89" s="15"/>
       <c r="T89" s="25" t="str">
@@ -9078,9 +9183,7 @@
       <c r="E90" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="G90" s="14" t="s">
-        <v>5</v>
-      </c>
+      <c r="G90" s="14"/>
       <c r="H90" s="19" t="str">
         <f t="shared" si="42"/>
         <v>Object</v>
@@ -9088,11 +9191,11 @@
       <c r="I90" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J90" s="21" t="s">
-        <v>602</v>
-      </c>
-      <c r="K90" s="22" t="s">
-        <v>603</v>
+      <c r="J90" s="52" t="s">
+        <v>543</v>
+      </c>
+      <c r="K90" s="52" t="s">
+        <v>544</v>
       </c>
       <c r="M90" s="14"/>
       <c r="N90" s="25" t="str">
@@ -9101,10 +9204,10 @@
       </c>
       <c r="O90" s="29"/>
       <c r="P90" s="27" t="s">
-        <v>410</v>
+        <v>621</v>
       </c>
       <c r="Q90" s="28" t="s">
-        <v>411</v>
+        <v>622</v>
       </c>
       <c r="S90" s="14"/>
       <c r="T90" s="25" t="str">
@@ -9164,10 +9267,10 @@
       <c r="I91" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="J91" s="21" t="s">
+      <c r="J91" s="52" t="s">
         <v>342</v>
       </c>
-      <c r="K91" s="22" t="s">
+      <c r="K91" s="52" t="s">
         <v>343</v>
       </c>
       <c r="M91" s="15"/>
@@ -9179,10 +9282,10 @@
         <v>5</v>
       </c>
       <c r="P91" s="23" t="s">
-        <v>508</v>
+        <v>458</v>
       </c>
       <c r="Q91" s="24" t="s">
-        <v>509</v>
+        <v>459</v>
       </c>
       <c r="S91" s="15"/>
       <c r="T91" s="19" t="str">
@@ -9252,9 +9355,7 @@
       <c r="E92" s="24" t="s">
         <v>218</v>
       </c>
-      <c r="G92" s="15" t="s">
-        <v>5</v>
-      </c>
+      <c r="G92" s="15"/>
       <c r="H92" s="19" t="str">
         <f t="shared" si="42"/>
         <v>TextObj</v>
@@ -9262,11 +9363,11 @@
       <c r="I92" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J92" s="21" t="s">
-        <v>581</v>
-      </c>
-      <c r="K92" s="22" t="s">
-        <v>582</v>
+      <c r="J92" s="52" t="s">
+        <v>522</v>
+      </c>
+      <c r="K92" s="52" t="s">
+        <v>523</v>
       </c>
       <c r="M92" s="15"/>
       <c r="N92" s="25" t="str">
@@ -9275,10 +9376,10 @@
       </c>
       <c r="O92" s="26"/>
       <c r="P92" s="27" t="s">
-        <v>561</v>
+        <v>502</v>
       </c>
       <c r="Q92" s="28" t="s">
-        <v>562</v>
+        <v>503</v>
       </c>
       <c r="S92" s="15"/>
       <c r="T92" s="19" t="str">
@@ -9338,10 +9439,10 @@
       <c r="I93" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J93" s="21" t="s">
+      <c r="J93" s="52" t="s">
         <v>344</v>
       </c>
-      <c r="K93" s="22" t="s">
+      <c r="K93" s="52" t="s">
         <v>345</v>
       </c>
       <c r="M93" s="15"/>
@@ -9353,10 +9454,10 @@
         <v>5</v>
       </c>
       <c r="P93" s="23" t="s">
-        <v>510</v>
+        <v>460</v>
       </c>
       <c r="Q93" s="24" t="s">
-        <v>511</v>
+        <v>461</v>
       </c>
       <c r="S93" s="15"/>
       <c r="T93" s="19" t="str">
@@ -9501,10 +9602,10 @@
         <v>BoolObj</v>
       </c>
       <c r="I95" s="26"/>
-      <c r="J95" s="27" t="s">
+      <c r="J95" s="51" t="s">
         <v>346</v>
       </c>
-      <c r="K95" s="28" t="s">
+      <c r="K95" s="51" t="s">
         <v>347</v>
       </c>
       <c r="M95" s="15"/>
@@ -9514,10 +9615,10 @@
       </c>
       <c r="O95" s="26"/>
       <c r="P95" s="27" t="s">
-        <v>512</v>
+        <v>462</v>
       </c>
       <c r="Q95" s="28" t="s">
-        <v>513</v>
+        <v>463</v>
       </c>
       <c r="S95" s="15"/>
       <c r="T95" s="25" t="str">
@@ -9571,10 +9672,10 @@
         <v>boolean</v>
       </c>
       <c r="I96" s="26"/>
-      <c r="J96" s="27" t="s">
+      <c r="J96" s="51" t="s">
         <v>348</v>
       </c>
-      <c r="K96" s="28" t="s">
+      <c r="K96" s="51" t="s">
         <v>349</v>
       </c>
       <c r="M96" s="15"/>
@@ -9584,10 +9685,10 @@
       </c>
       <c r="O96" s="26"/>
       <c r="P96" s="27" t="s">
-        <v>514</v>
+        <v>464</v>
       </c>
       <c r="Q96" s="28" t="s">
-        <v>515</v>
+        <v>465</v>
       </c>
       <c r="S96" s="15"/>
       <c r="T96" s="25" t="str">
@@ -9645,10 +9746,10 @@
         <v>IntObj</v>
       </c>
       <c r="I97" s="26"/>
-      <c r="J97" s="27" t="s">
+      <c r="J97" s="51" t="s">
         <v>350</v>
       </c>
-      <c r="K97" s="28" t="s">
+      <c r="K97" s="51" t="s">
         <v>351</v>
       </c>
       <c r="M97" s="15"/>
@@ -9658,10 +9759,10 @@
       </c>
       <c r="O97" s="26"/>
       <c r="P97" s="27" t="s">
-        <v>516</v>
+        <v>466</v>
       </c>
       <c r="Q97" s="28" t="s">
-        <v>517</v>
+        <v>467</v>
       </c>
       <c r="S97" s="15"/>
       <c r="T97" s="25" t="str">
@@ -9715,10 +9816,10 @@
         <v>integer</v>
       </c>
       <c r="I98" s="26"/>
-      <c r="J98" s="27" t="s">
+      <c r="J98" s="51" t="s">
         <v>352</v>
       </c>
-      <c r="K98" s="28" t="s">
+      <c r="K98" s="51" t="s">
         <v>353</v>
       </c>
       <c r="M98" s="15"/>
@@ -9728,10 +9829,10 @@
       </c>
       <c r="O98" s="26"/>
       <c r="P98" s="27" t="s">
-        <v>518</v>
+        <v>468</v>
       </c>
       <c r="Q98" s="28" t="s">
-        <v>519</v>
+        <v>469</v>
       </c>
       <c r="S98" s="15"/>
       <c r="T98" s="25" t="str">
@@ -9787,10 +9888,10 @@
         <v>NumObj</v>
       </c>
       <c r="I99" s="26"/>
-      <c r="J99" s="27" t="s">
+      <c r="J99" s="51" t="s">
         <v>354</v>
       </c>
-      <c r="K99" s="28" t="s">
+      <c r="K99" s="51" t="s">
         <v>355</v>
       </c>
       <c r="M99" s="15"/>
@@ -9800,10 +9901,10 @@
       </c>
       <c r="O99" s="26"/>
       <c r="P99" s="27" t="s">
-        <v>520</v>
+        <v>470</v>
       </c>
       <c r="Q99" s="28" t="s">
-        <v>521</v>
+        <v>471</v>
       </c>
       <c r="S99" s="15"/>
       <c r="T99" s="25" t="str">
@@ -9857,10 +9958,10 @@
         <v>number</v>
       </c>
       <c r="I100" s="26"/>
-      <c r="J100" s="27" t="s">
+      <c r="J100" s="51" t="s">
         <v>356</v>
       </c>
-      <c r="K100" s="28" t="s">
+      <c r="K100" s="51" t="s">
         <v>357</v>
       </c>
       <c r="M100" s="15"/>
@@ -9870,10 +9971,10 @@
       </c>
       <c r="O100" s="26"/>
       <c r="P100" s="27" t="s">
-        <v>522</v>
+        <v>472</v>
       </c>
       <c r="Q100" s="28" t="s">
-        <v>523</v>
+        <v>473</v>
       </c>
       <c r="S100" s="15"/>
       <c r="T100" s="25" t="str">
@@ -9925,9 +10026,7 @@
       <c r="E101" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="G101" s="14" t="s">
-        <v>5</v>
-      </c>
+      <c r="G101" s="14"/>
       <c r="H101" s="19" t="str">
         <f t="shared" si="48"/>
         <v>Object</v>
@@ -9935,11 +10034,11 @@
       <c r="I101" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J101" s="21" t="s">
-        <v>604</v>
-      </c>
-      <c r="K101" s="22" t="s">
-        <v>605</v>
+      <c r="J101" s="52" t="s">
+        <v>545</v>
+      </c>
+      <c r="K101" s="52" t="s">
+        <v>546</v>
       </c>
       <c r="M101" s="14"/>
       <c r="N101" s="25" t="str">
@@ -9948,10 +10047,10 @@
       </c>
       <c r="O101" s="29"/>
       <c r="P101" s="27" t="s">
-        <v>412</v>
+        <v>623</v>
       </c>
       <c r="Q101" s="28" t="s">
-        <v>413</v>
+        <v>624</v>
       </c>
       <c r="S101" s="14"/>
       <c r="T101" s="25" t="str">
@@ -10004,16 +10103,18 @@
         <v>212</v>
       </c>
       <c r="G102" s="15"/>
-      <c r="H102" s="25" t="str">
+      <c r="H102" s="19" t="str">
         <f t="shared" si="48"/>
         <v>text</v>
       </c>
-      <c r="I102" s="26"/>
-      <c r="J102" s="27" t="s">
-        <v>557</v>
-      </c>
-      <c r="K102" s="28" t="s">
-        <v>558</v>
+      <c r="I102" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J102" s="52" t="s">
+        <v>639</v>
+      </c>
+      <c r="K102" s="52" t="s">
+        <v>640</v>
       </c>
       <c r="M102" s="15"/>
       <c r="N102" s="25" t="str">
@@ -10022,10 +10123,10 @@
       </c>
       <c r="O102" s="26"/>
       <c r="P102" s="27" t="s">
-        <v>559</v>
+        <v>500</v>
       </c>
       <c r="Q102" s="28" t="s">
-        <v>560</v>
+        <v>501</v>
       </c>
       <c r="S102" s="15"/>
       <c r="T102" s="19" t="str">
@@ -10085,10 +10186,10 @@
       <c r="I103" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="J103" s="21" t="s">
+      <c r="J103" s="52" t="s">
         <v>358</v>
       </c>
-      <c r="K103" s="22" t="s">
+      <c r="K103" s="52" t="s">
         <v>359</v>
       </c>
       <c r="M103" s="15"/>
@@ -10100,10 +10201,10 @@
         <v>5</v>
       </c>
       <c r="P103" s="23" t="s">
-        <v>524</v>
+        <v>474</v>
       </c>
       <c r="Q103" s="24" t="s">
-        <v>525</v>
+        <v>475</v>
       </c>
       <c r="S103" s="15"/>
       <c r="T103" s="19" t="str">
@@ -10163,10 +10264,10 @@
       <c r="I104" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J104" s="21" t="s">
+      <c r="J104" s="52" t="s">
         <v>360</v>
       </c>
-      <c r="K104" s="22" t="s">
+      <c r="K104" s="52" t="s">
         <v>361</v>
       </c>
       <c r="M104" s="15"/>
@@ -10178,10 +10279,10 @@
         <v>5</v>
       </c>
       <c r="P104" s="23" t="s">
-        <v>526</v>
+        <v>476</v>
       </c>
       <c r="Q104" s="24" t="s">
-        <v>527</v>
+        <v>477</v>
       </c>
       <c r="S104" s="15"/>
       <c r="T104" s="19" t="str">
@@ -10308,10 +10409,10 @@
         <v>Object</v>
       </c>
       <c r="I106" s="33"/>
-      <c r="J106" s="27" t="s">
+      <c r="J106" s="51" t="s">
         <v>362</v>
       </c>
-      <c r="K106" s="28" t="s">
+      <c r="K106" s="51" t="s">
         <v>363</v>
       </c>
       <c r="M106" s="18"/>
@@ -10321,10 +10422,10 @@
       </c>
       <c r="O106" s="33"/>
       <c r="P106" s="34" t="s">
-        <v>528</v>
+        <v>478</v>
       </c>
       <c r="Q106" s="35" t="s">
-        <v>529</v>
+        <v>479</v>
       </c>
       <c r="S106" s="18"/>
       <c r="T106" s="32" t="str">
@@ -10803,186 +10904,186 @@
     <hyperlink ref="Q100" r:id="rId364" display="Fail\ExpAssignTextObjNumberField.quorum"/>
     <hyperlink ref="J7" r:id="rId365"/>
     <hyperlink ref="K7" r:id="rId366"/>
-    <hyperlink ref="J8" r:id="rId367"/>
-    <hyperlink ref="K8" r:id="rId368"/>
-    <hyperlink ref="J9" r:id="rId369"/>
-    <hyperlink ref="K9" r:id="rId370"/>
-    <hyperlink ref="J10" r:id="rId371"/>
-    <hyperlink ref="K10" r:id="rId372"/>
-    <hyperlink ref="J11" r:id="rId373"/>
-    <hyperlink ref="K11" r:id="rId374"/>
-    <hyperlink ref="J12" r:id="rId375"/>
-    <hyperlink ref="K12" r:id="rId376"/>
-    <hyperlink ref="J13" r:id="rId377"/>
-    <hyperlink ref="K13" r:id="rId378"/>
-    <hyperlink ref="J14" r:id="rId379"/>
-    <hyperlink ref="K14" r:id="rId380"/>
-    <hyperlink ref="J15" r:id="rId381"/>
-    <hyperlink ref="K15" r:id="rId382"/>
-    <hyperlink ref="J16" r:id="rId383"/>
-    <hyperlink ref="K16" r:id="rId384"/>
-    <hyperlink ref="J18" r:id="rId385"/>
-    <hyperlink ref="K18" r:id="rId386"/>
-    <hyperlink ref="J19" r:id="rId387"/>
-    <hyperlink ref="K19" r:id="rId388"/>
-    <hyperlink ref="J20" r:id="rId389"/>
-    <hyperlink ref="K20" r:id="rId390"/>
-    <hyperlink ref="J21" r:id="rId391"/>
-    <hyperlink ref="K21" r:id="rId392"/>
-    <hyperlink ref="J22" r:id="rId393"/>
-    <hyperlink ref="K22" r:id="rId394"/>
-    <hyperlink ref="J23" r:id="rId395"/>
-    <hyperlink ref="K23" r:id="rId396"/>
-    <hyperlink ref="J24" r:id="rId397"/>
-    <hyperlink ref="K24" r:id="rId398"/>
-    <hyperlink ref="J25" r:id="rId399"/>
-    <hyperlink ref="K25" r:id="rId400"/>
-    <hyperlink ref="J26" r:id="rId401"/>
-    <hyperlink ref="K26" r:id="rId402"/>
-    <hyperlink ref="J27" r:id="rId403"/>
-    <hyperlink ref="K27" r:id="rId404"/>
-    <hyperlink ref="J29" r:id="rId405"/>
-    <hyperlink ref="K29" r:id="rId406"/>
-    <hyperlink ref="J30" r:id="rId407"/>
-    <hyperlink ref="K30" r:id="rId408"/>
-    <hyperlink ref="J31" r:id="rId409"/>
-    <hyperlink ref="K31" r:id="rId410"/>
-    <hyperlink ref="J32" r:id="rId411"/>
-    <hyperlink ref="K32" r:id="rId412"/>
-    <hyperlink ref="J33" r:id="rId413"/>
-    <hyperlink ref="K33" r:id="rId414"/>
-    <hyperlink ref="J34" r:id="rId415"/>
-    <hyperlink ref="K34" r:id="rId416"/>
-    <hyperlink ref="J35" r:id="rId417"/>
-    <hyperlink ref="K35" r:id="rId418"/>
-    <hyperlink ref="J36" r:id="rId419"/>
-    <hyperlink ref="K36" r:id="rId420"/>
-    <hyperlink ref="J37" r:id="rId421"/>
-    <hyperlink ref="K37" r:id="rId422"/>
-    <hyperlink ref="J38" r:id="rId423"/>
-    <hyperlink ref="K38" r:id="rId424"/>
-    <hyperlink ref="J40" r:id="rId425"/>
-    <hyperlink ref="K40" r:id="rId426"/>
-    <hyperlink ref="J41" r:id="rId427"/>
-    <hyperlink ref="K41" r:id="rId428"/>
-    <hyperlink ref="J42" r:id="rId429"/>
-    <hyperlink ref="K42" r:id="rId430"/>
-    <hyperlink ref="J43" r:id="rId431"/>
-    <hyperlink ref="K43" r:id="rId432"/>
-    <hyperlink ref="J44" r:id="rId433"/>
-    <hyperlink ref="K44" r:id="rId434"/>
-    <hyperlink ref="J45" r:id="rId435"/>
-    <hyperlink ref="K45" r:id="rId436"/>
-    <hyperlink ref="J46" r:id="rId437"/>
-    <hyperlink ref="K46" r:id="rId438"/>
-    <hyperlink ref="J47" r:id="rId439"/>
-    <hyperlink ref="K47" r:id="rId440"/>
-    <hyperlink ref="J48" r:id="rId441"/>
-    <hyperlink ref="K48" r:id="rId442"/>
-    <hyperlink ref="J49" r:id="rId443"/>
-    <hyperlink ref="K49" r:id="rId444"/>
-    <hyperlink ref="J51" r:id="rId445"/>
-    <hyperlink ref="K51" r:id="rId446"/>
-    <hyperlink ref="J52" r:id="rId447"/>
-    <hyperlink ref="K52" r:id="rId448"/>
-    <hyperlink ref="J53" r:id="rId449"/>
-    <hyperlink ref="K53" r:id="rId450"/>
-    <hyperlink ref="J54" r:id="rId451"/>
-    <hyperlink ref="K54" r:id="rId452"/>
-    <hyperlink ref="J55" r:id="rId453"/>
-    <hyperlink ref="K55" r:id="rId454"/>
-    <hyperlink ref="J56" r:id="rId455"/>
-    <hyperlink ref="K56" r:id="rId456"/>
-    <hyperlink ref="J57" r:id="rId457"/>
-    <hyperlink ref="K57" r:id="rId458"/>
-    <hyperlink ref="J58" r:id="rId459"/>
-    <hyperlink ref="K58" r:id="rId460"/>
-    <hyperlink ref="J59" r:id="rId461"/>
-    <hyperlink ref="K59" r:id="rId462"/>
-    <hyperlink ref="J60" r:id="rId463"/>
-    <hyperlink ref="K60" r:id="rId464"/>
-    <hyperlink ref="J62" r:id="rId465"/>
-    <hyperlink ref="K62" r:id="rId466"/>
-    <hyperlink ref="J63" r:id="rId467"/>
-    <hyperlink ref="K63" r:id="rId468"/>
-    <hyperlink ref="J64" r:id="rId469"/>
-    <hyperlink ref="K64" r:id="rId470"/>
-    <hyperlink ref="J65" r:id="rId471"/>
-    <hyperlink ref="K65" r:id="rId472"/>
-    <hyperlink ref="J66" r:id="rId473"/>
-    <hyperlink ref="K66" r:id="rId474"/>
-    <hyperlink ref="J67" r:id="rId475"/>
-    <hyperlink ref="K67" r:id="rId476"/>
-    <hyperlink ref="J68" r:id="rId477"/>
-    <hyperlink ref="K68" r:id="rId478"/>
-    <hyperlink ref="J69" r:id="rId479"/>
-    <hyperlink ref="K69" r:id="rId480"/>
-    <hyperlink ref="J70" r:id="rId481"/>
-    <hyperlink ref="K70" r:id="rId482"/>
-    <hyperlink ref="J71" r:id="rId483"/>
-    <hyperlink ref="K71" r:id="rId484"/>
-    <hyperlink ref="J73" r:id="rId485"/>
-    <hyperlink ref="K73" r:id="rId486"/>
-    <hyperlink ref="J74" r:id="rId487"/>
-    <hyperlink ref="K74" r:id="rId488"/>
-    <hyperlink ref="J75" r:id="rId489"/>
-    <hyperlink ref="K75" r:id="rId490"/>
-    <hyperlink ref="J76" r:id="rId491"/>
-    <hyperlink ref="K76" r:id="rId492"/>
-    <hyperlink ref="J77" r:id="rId493"/>
-    <hyperlink ref="K77" r:id="rId494"/>
-    <hyperlink ref="J78" r:id="rId495"/>
-    <hyperlink ref="K78" r:id="rId496"/>
-    <hyperlink ref="J79" r:id="rId497"/>
-    <hyperlink ref="K79" r:id="rId498"/>
-    <hyperlink ref="J80" r:id="rId499"/>
-    <hyperlink ref="K80" r:id="rId500"/>
-    <hyperlink ref="J81" r:id="rId501"/>
-    <hyperlink ref="K81" r:id="rId502"/>
-    <hyperlink ref="J82" r:id="rId503"/>
-    <hyperlink ref="K82" r:id="rId504"/>
-    <hyperlink ref="J84" r:id="rId505"/>
-    <hyperlink ref="K84" r:id="rId506"/>
-    <hyperlink ref="J85" r:id="rId507"/>
-    <hyperlink ref="K85" r:id="rId508"/>
-    <hyperlink ref="J86" r:id="rId509"/>
-    <hyperlink ref="K86" r:id="rId510"/>
-    <hyperlink ref="J87" r:id="rId511"/>
-    <hyperlink ref="K87" r:id="rId512"/>
-    <hyperlink ref="J88" r:id="rId513"/>
-    <hyperlink ref="K88" r:id="rId514"/>
-    <hyperlink ref="J89" r:id="rId515"/>
-    <hyperlink ref="K89" r:id="rId516"/>
-    <hyperlink ref="J90" r:id="rId517"/>
-    <hyperlink ref="K90" r:id="rId518"/>
-    <hyperlink ref="J91" r:id="rId519"/>
-    <hyperlink ref="K91" r:id="rId520"/>
-    <hyperlink ref="J92" r:id="rId521"/>
-    <hyperlink ref="K92" r:id="rId522"/>
-    <hyperlink ref="J93" r:id="rId523"/>
-    <hyperlink ref="K93" r:id="rId524"/>
-    <hyperlink ref="J95" r:id="rId525"/>
-    <hyperlink ref="K95" r:id="rId526"/>
-    <hyperlink ref="J96" r:id="rId527"/>
-    <hyperlink ref="K96" r:id="rId528"/>
-    <hyperlink ref="J97" r:id="rId529"/>
-    <hyperlink ref="K97" r:id="rId530"/>
-    <hyperlink ref="J98" r:id="rId531"/>
-    <hyperlink ref="K98" r:id="rId532"/>
-    <hyperlink ref="J99" r:id="rId533"/>
-    <hyperlink ref="K99" r:id="rId534"/>
-    <hyperlink ref="J100" r:id="rId535"/>
-    <hyperlink ref="K100" r:id="rId536"/>
-    <hyperlink ref="J101" r:id="rId537"/>
-    <hyperlink ref="K101" r:id="rId538"/>
-    <hyperlink ref="J102" r:id="rId539"/>
-    <hyperlink ref="K102" r:id="rId540"/>
-    <hyperlink ref="J103" r:id="rId541"/>
-    <hyperlink ref="K103" r:id="rId542"/>
-    <hyperlink ref="J104" r:id="rId543"/>
-    <hyperlink ref="K104" r:id="rId544"/>
-    <hyperlink ref="J106" r:id="rId545"/>
-    <hyperlink ref="K106" r:id="rId546"/>
+    <hyperlink ref="J9" r:id="rId367"/>
+    <hyperlink ref="K9" r:id="rId368"/>
+    <hyperlink ref="J10" r:id="rId369"/>
+    <hyperlink ref="K10" r:id="rId370"/>
+    <hyperlink ref="J11" r:id="rId371"/>
+    <hyperlink ref="K11" r:id="rId372"/>
+    <hyperlink ref="J12" r:id="rId373"/>
+    <hyperlink ref="K12" r:id="rId374"/>
+    <hyperlink ref="J13" r:id="rId375"/>
+    <hyperlink ref="K13" r:id="rId376"/>
+    <hyperlink ref="J14" r:id="rId377"/>
+    <hyperlink ref="K14" r:id="rId378"/>
+    <hyperlink ref="J15" r:id="rId379"/>
+    <hyperlink ref="K15" r:id="rId380"/>
+    <hyperlink ref="J16" r:id="rId381"/>
+    <hyperlink ref="K16" r:id="rId382"/>
+    <hyperlink ref="J18" r:id="rId383"/>
+    <hyperlink ref="K18" r:id="rId384"/>
+    <hyperlink ref="J19" r:id="rId385"/>
+    <hyperlink ref="K19" r:id="rId386"/>
+    <hyperlink ref="J20" r:id="rId387"/>
+    <hyperlink ref="K20" r:id="rId388"/>
+    <hyperlink ref="J21" r:id="rId389"/>
+    <hyperlink ref="K21" r:id="rId390"/>
+    <hyperlink ref="J22" r:id="rId391"/>
+    <hyperlink ref="K22" r:id="rId392"/>
+    <hyperlink ref="J23" r:id="rId393"/>
+    <hyperlink ref="K23" r:id="rId394"/>
+    <hyperlink ref="J24" r:id="rId395"/>
+    <hyperlink ref="K24" r:id="rId396"/>
+    <hyperlink ref="J25" r:id="rId397"/>
+    <hyperlink ref="K25" r:id="rId398"/>
+    <hyperlink ref="J26" r:id="rId399"/>
+    <hyperlink ref="K26" r:id="rId400"/>
+    <hyperlink ref="J27" r:id="rId401"/>
+    <hyperlink ref="K27" r:id="rId402"/>
+    <hyperlink ref="J29" r:id="rId403"/>
+    <hyperlink ref="K29" r:id="rId404"/>
+    <hyperlink ref="J30" r:id="rId405"/>
+    <hyperlink ref="K30" r:id="rId406"/>
+    <hyperlink ref="J31" r:id="rId407"/>
+    <hyperlink ref="K31" r:id="rId408"/>
+    <hyperlink ref="J33" r:id="rId409"/>
+    <hyperlink ref="K33" r:id="rId410"/>
+    <hyperlink ref="J34" r:id="rId411"/>
+    <hyperlink ref="K34" r:id="rId412"/>
+    <hyperlink ref="J35" r:id="rId413"/>
+    <hyperlink ref="K35" r:id="rId414"/>
+    <hyperlink ref="J36" r:id="rId415"/>
+    <hyperlink ref="K36" r:id="rId416"/>
+    <hyperlink ref="J37" r:id="rId417"/>
+    <hyperlink ref="K37" r:id="rId418"/>
+    <hyperlink ref="J38" r:id="rId419"/>
+    <hyperlink ref="K38" r:id="rId420"/>
+    <hyperlink ref="J40" r:id="rId421"/>
+    <hyperlink ref="K40" r:id="rId422"/>
+    <hyperlink ref="J41" r:id="rId423"/>
+    <hyperlink ref="K41" r:id="rId424"/>
+    <hyperlink ref="J42" r:id="rId425"/>
+    <hyperlink ref="K42" r:id="rId426"/>
+    <hyperlink ref="J43" r:id="rId427"/>
+    <hyperlink ref="K43" r:id="rId428"/>
+    <hyperlink ref="J44" r:id="rId429"/>
+    <hyperlink ref="K44" r:id="rId430"/>
+    <hyperlink ref="J45" r:id="rId431"/>
+    <hyperlink ref="K45" r:id="rId432"/>
+    <hyperlink ref="J46" r:id="rId433"/>
+    <hyperlink ref="K46" r:id="rId434"/>
+    <hyperlink ref="J47" r:id="rId435"/>
+    <hyperlink ref="K47" r:id="rId436"/>
+    <hyperlink ref="J48" r:id="rId437"/>
+    <hyperlink ref="K48" r:id="rId438"/>
+    <hyperlink ref="J49" r:id="rId439"/>
+    <hyperlink ref="K49" r:id="rId440"/>
+    <hyperlink ref="J51" r:id="rId441"/>
+    <hyperlink ref="K51" r:id="rId442"/>
+    <hyperlink ref="J52" r:id="rId443"/>
+    <hyperlink ref="K52" r:id="rId444"/>
+    <hyperlink ref="J53" r:id="rId445"/>
+    <hyperlink ref="K53" r:id="rId446"/>
+    <hyperlink ref="J54" r:id="rId447"/>
+    <hyperlink ref="K54" r:id="rId448"/>
+    <hyperlink ref="J55" r:id="rId449"/>
+    <hyperlink ref="K55" r:id="rId450"/>
+    <hyperlink ref="J57" r:id="rId451"/>
+    <hyperlink ref="K57" r:id="rId452"/>
+    <hyperlink ref="J58" r:id="rId453"/>
+    <hyperlink ref="K58" r:id="rId454"/>
+    <hyperlink ref="J59" r:id="rId455"/>
+    <hyperlink ref="K59" r:id="rId456"/>
+    <hyperlink ref="J60" r:id="rId457"/>
+    <hyperlink ref="K60" r:id="rId458"/>
+    <hyperlink ref="J62" r:id="rId459"/>
+    <hyperlink ref="K62" r:id="rId460"/>
+    <hyperlink ref="J63" r:id="rId461"/>
+    <hyperlink ref="K63" r:id="rId462"/>
+    <hyperlink ref="J64" r:id="rId463"/>
+    <hyperlink ref="K64" r:id="rId464"/>
+    <hyperlink ref="J65" r:id="rId465"/>
+    <hyperlink ref="K65" r:id="rId466"/>
+    <hyperlink ref="J66" r:id="rId467"/>
+    <hyperlink ref="K66" r:id="rId468"/>
+    <hyperlink ref="J67" r:id="rId469"/>
+    <hyperlink ref="K67" r:id="rId470"/>
+    <hyperlink ref="J68" r:id="rId471"/>
+    <hyperlink ref="K68" r:id="rId472"/>
+    <hyperlink ref="J69" r:id="rId473"/>
+    <hyperlink ref="K69" r:id="rId474"/>
+    <hyperlink ref="J70" r:id="rId475"/>
+    <hyperlink ref="K70" r:id="rId476"/>
+    <hyperlink ref="J71" r:id="rId477"/>
+    <hyperlink ref="K71" r:id="rId478"/>
+    <hyperlink ref="J73" r:id="rId479"/>
+    <hyperlink ref="K73" r:id="rId480"/>
+    <hyperlink ref="J75" r:id="rId481"/>
+    <hyperlink ref="K75" r:id="rId482"/>
+    <hyperlink ref="J77" r:id="rId483"/>
+    <hyperlink ref="K77" r:id="rId484"/>
+    <hyperlink ref="J79" r:id="rId485"/>
+    <hyperlink ref="K79" r:id="rId486"/>
+    <hyperlink ref="J81" r:id="rId487"/>
+    <hyperlink ref="K81" r:id="rId488"/>
+    <hyperlink ref="J82" r:id="rId489"/>
+    <hyperlink ref="K82" r:id="rId490"/>
+    <hyperlink ref="J84" r:id="rId491"/>
+    <hyperlink ref="K84" r:id="rId492"/>
+    <hyperlink ref="J85" r:id="rId493"/>
+    <hyperlink ref="K85" r:id="rId494"/>
+    <hyperlink ref="J86" r:id="rId495"/>
+    <hyperlink ref="K86" r:id="rId496"/>
+    <hyperlink ref="J87" r:id="rId497"/>
+    <hyperlink ref="K87" r:id="rId498"/>
+    <hyperlink ref="J88" r:id="rId499"/>
+    <hyperlink ref="K88" r:id="rId500"/>
+    <hyperlink ref="J89" r:id="rId501"/>
+    <hyperlink ref="K89" r:id="rId502"/>
+    <hyperlink ref="J90" r:id="rId503"/>
+    <hyperlink ref="K90" r:id="rId504"/>
+    <hyperlink ref="J91" r:id="rId505"/>
+    <hyperlink ref="K91" r:id="rId506"/>
+    <hyperlink ref="J92" r:id="rId507"/>
+    <hyperlink ref="K92" r:id="rId508"/>
+    <hyperlink ref="J93" r:id="rId509"/>
+    <hyperlink ref="K93" r:id="rId510"/>
+    <hyperlink ref="J95" r:id="rId511"/>
+    <hyperlink ref="K95" r:id="rId512"/>
+    <hyperlink ref="J96" r:id="rId513"/>
+    <hyperlink ref="K96" r:id="rId514"/>
+    <hyperlink ref="J97" r:id="rId515"/>
+    <hyperlink ref="K97" r:id="rId516"/>
+    <hyperlink ref="J98" r:id="rId517"/>
+    <hyperlink ref="K98" r:id="rId518"/>
+    <hyperlink ref="J99" r:id="rId519"/>
+    <hyperlink ref="K99" r:id="rId520"/>
+    <hyperlink ref="J100" r:id="rId521"/>
+    <hyperlink ref="K100" r:id="rId522"/>
+    <hyperlink ref="J101" r:id="rId523"/>
+    <hyperlink ref="K101" r:id="rId524"/>
+    <hyperlink ref="J103" r:id="rId525"/>
+    <hyperlink ref="K103" r:id="rId526"/>
+    <hyperlink ref="J104" r:id="rId527"/>
+    <hyperlink ref="K104" r:id="rId528"/>
+    <hyperlink ref="J106" r:id="rId529"/>
+    <hyperlink ref="K106" r:id="rId530"/>
+    <hyperlink ref="J8" r:id="rId531"/>
+    <hyperlink ref="K8" r:id="rId532"/>
+    <hyperlink ref="J32" r:id="rId533"/>
+    <hyperlink ref="K32" r:id="rId534"/>
+    <hyperlink ref="J56" r:id="rId535"/>
+    <hyperlink ref="K56" r:id="rId536"/>
+    <hyperlink ref="J74" r:id="rId537"/>
+    <hyperlink ref="K74" r:id="rId538"/>
+    <hyperlink ref="K76" r:id="rId539"/>
+    <hyperlink ref="J76" r:id="rId540"/>
+    <hyperlink ref="J78" r:id="rId541"/>
+    <hyperlink ref="K78" r:id="rId542"/>
+    <hyperlink ref="K80" r:id="rId543"/>
+    <hyperlink ref="J80" r:id="rId544"/>
+    <hyperlink ref="J102" r:id="rId545"/>
+    <hyperlink ref="K102" r:id="rId546"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId547"/>
@@ -11007,42 +11108,42 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>414</v>
+        <v>364</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>415</v>
+        <v>365</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>416</v>
+        <v>366</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>417</v>
+        <v>367</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>418</v>
+        <v>368</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>419</v>
+        <v>369</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>420</v>
+        <v>370</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>421</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -11163,11 +11264,11 @@
       </c>
       <c r="H4" t="str">
         <f>IF('Quorum 3.0'!I8="x", "Pass", "Fail")</f>
-        <v>Fail</v>
+        <v>Pass</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" ref="I4:I67" si="1">F4&amp;","&amp;G4&amp;","&amp;H4</f>
-        <v>BoolObj,boolean,Fail</v>
+        <v>BoolObj,boolean,Pass</v>
       </c>
       <c r="K4" t="str">
         <f>'Quorum 3.0'!M$6</f>
@@ -11613,11 +11714,11 @@
       </c>
       <c r="H13" t="str">
         <f>IF('Quorum 3.0'!I18="x", "Pass", "Fail")</f>
-        <v>Fail</v>
+        <v>Pass</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="1"/>
-        <v>boolean,BoolObj,Fail</v>
+        <v>boolean,BoolObj,Pass</v>
       </c>
       <c r="K13" t="str">
         <f>'Quorum 3.0'!M$17</f>
@@ -12263,11 +12364,11 @@
       </c>
       <c r="H26" t="str">
         <f>IF('Quorum 3.0'!I32="x", "Pass", "Fail")</f>
-        <v>Fail</v>
+        <v>Pass</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="1"/>
-        <v>IntObj,integer,Fail</v>
+        <v>IntObj,integer,Pass</v>
       </c>
       <c r="K26" t="str">
         <f>'Quorum 3.0'!M$28</f>
@@ -13363,11 +13464,11 @@
       </c>
       <c r="H48" t="str">
         <f>IF('Quorum 3.0'!I56="x", "Pass", "Fail")</f>
-        <v>Fail</v>
+        <v>Pass</v>
       </c>
       <c r="I48" t="str">
         <f t="shared" si="1"/>
-        <v>NumObj,number,Fail</v>
+        <v>NumObj,number,Pass</v>
       </c>
       <c r="K48" t="str">
         <f>'Quorum 3.0'!M$50</f>
@@ -14163,11 +14264,11 @@
       </c>
       <c r="H64" t="str">
         <f>IF('Quorum 3.0'!I74="x", "Pass", "Fail")</f>
-        <v>Fail</v>
+        <v>Pass</v>
       </c>
       <c r="I64" t="str">
         <f t="shared" si="1"/>
-        <v>Object,boolean,Fail</v>
+        <v>Object,boolean,Pass</v>
       </c>
       <c r="K64" t="str">
         <f>'Quorum 3.0'!M$72</f>
@@ -14263,11 +14364,11 @@
       </c>
       <c r="H66" t="str">
         <f>IF('Quorum 3.0'!I76="x", "Pass", "Fail")</f>
-        <v>Fail</v>
+        <v>Pass</v>
       </c>
       <c r="I66" t="str">
         <f t="shared" si="1"/>
-        <v>Object,integer,Fail</v>
+        <v>Object,integer,Pass</v>
       </c>
       <c r="K66" t="str">
         <f>'Quorum 3.0'!M$72</f>
@@ -14363,11 +14464,11 @@
       </c>
       <c r="H68" t="str">
         <f>IF('Quorum 3.0'!I78="x", "Pass", "Fail")</f>
-        <v>Fail</v>
+        <v>Pass</v>
       </c>
       <c r="I68" t="str">
         <f t="shared" ref="I68:I93" si="4">F68&amp;","&amp;G68&amp;","&amp;H68</f>
-        <v>Object,number,Fail</v>
+        <v>Object,number,Pass</v>
       </c>
       <c r="K68" t="str">
         <f>'Quorum 3.0'!M$72</f>
@@ -14463,11 +14564,11 @@
       </c>
       <c r="H70" t="str">
         <f>IF('Quorum 3.0'!I80="x", "Pass", "Fail")</f>
-        <v>Fail</v>
+        <v>Pass</v>
       </c>
       <c r="I70" t="str">
         <f t="shared" si="4"/>
-        <v>Object,text,Fail</v>
+        <v>Object,text,Pass</v>
       </c>
       <c r="K70" t="str">
         <f>'Quorum 3.0'!M$72</f>
@@ -15463,11 +15564,11 @@
       </c>
       <c r="H90" t="str">
         <f>IF('Quorum 3.0'!I102="x", "Pass", "Fail")</f>
-        <v>Fail</v>
+        <v>Pass</v>
       </c>
       <c r="I90" t="str">
         <f t="shared" si="4"/>
-        <v>TextObj,text,Fail</v>
+        <v>TextObj,text,Pass</v>
       </c>
       <c r="K90" t="str">
         <f>'Quorum 3.0'!M$94</f>

</xml_diff>

<commit_message>
TypeCheck TextUndefined moved to Fail
</commit_message>
<xml_diff>
--- a/Quorum3/Library/Tests/TypeCheckerGenerated/Type System.xlsx
+++ b/Quorum3/Library/Tests/TypeCheckerGenerated/Type System.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="600" windowWidth="29580" windowHeight="16440"/>
+    <workbookView xWindow="645" yWindow="600" windowWidth="29580" windowHeight="16440" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Quorum 3.0" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="640">
   <si>
     <t>Type System</t>
   </si>
@@ -1055,12 +1055,6 @@
     <t>Pass\ImpAssignTextTextField.quorum</t>
   </si>
   <si>
-    <t>Pass\ImpAssignTextUndefined.quorum</t>
-  </si>
-  <si>
-    <t>Pass\ImpAssignTextUndefinedField.quorum</t>
-  </si>
-  <si>
     <t>Fail\ImpAssignTextObjBoolObj.quorum</t>
   </si>
   <si>
@@ -1941,6 +1935,12 @@
   </si>
   <si>
     <t>Fail\ImpAssignIntegerNumObjField.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignTextUndefined.quorum</t>
+  </si>
+  <si>
+    <t>Fail\ImpAssignTextUndefinedField.quorum</t>
   </si>
 </sst>
 </file>
@@ -2570,9 +2570,9 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AW114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="200" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="200" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I93" sqref="I93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2622,7 +2622,7 @@
     </row>
     <row r="2" spans="1:49" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B2" s="1"/>
       <c r="J2" s="3">
@@ -2635,7 +2635,7 @@
     </row>
     <row r="4" spans="1:49" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B4" s="47"/>
       <c r="C4" s="48"/>
@@ -2643,7 +2643,7 @@
       <c r="E4" s="49"/>
       <c r="F4" s="3"/>
       <c r="G4" s="46" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="H4" s="47"/>
       <c r="I4" s="48"/>
@@ -2651,7 +2651,7 @@
       <c r="K4" s="49"/>
       <c r="L4" s="3"/>
       <c r="M4" s="46" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="N4" s="47"/>
       <c r="O4" s="48"/>
@@ -2701,10 +2701,10 @@
         <v>105</v>
       </c>
       <c r="D5" s="44" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="E5" s="45" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="G5" s="42" t="str">
         <f>A5</f>
@@ -2943,10 +2943,10 @@
         <v>5</v>
       </c>
       <c r="P7" s="21" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="Q7" s="22" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="S7" s="15"/>
       <c r="T7" s="19" t="str">
@@ -3007,10 +3007,10 @@
         <v>5</v>
       </c>
       <c r="J8" s="52" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="K8" s="52" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="M8" s="15"/>
       <c r="N8" s="25" t="str">
@@ -3019,10 +3019,10 @@
       </c>
       <c r="O8" s="26"/>
       <c r="P8" s="27" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="Q8" s="28" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="S8" s="15"/>
       <c r="T8" s="19" t="str">
@@ -3093,10 +3093,10 @@
       </c>
       <c r="O9" s="26"/>
       <c r="P9" s="27" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="Q9" s="28" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="S9" s="15"/>
       <c r="T9" s="25" t="str">
@@ -3163,10 +3163,10 @@
       </c>
       <c r="O10" s="29"/>
       <c r="P10" s="27" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="Q10" s="28" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="S10" s="15"/>
       <c r="T10" s="25" t="str">
@@ -3235,10 +3235,10 @@
       </c>
       <c r="O11" s="29"/>
       <c r="P11" s="27" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="Q11" s="28" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="S11" s="15"/>
       <c r="T11" s="25" t="str">
@@ -3307,10 +3307,10 @@
       </c>
       <c r="O12" s="29"/>
       <c r="P12" s="27" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="Q12" s="28" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="S12" s="15"/>
       <c r="T12" s="25" t="str">
@@ -3369,10 +3369,10 @@
       </c>
       <c r="I13" s="29"/>
       <c r="J13" s="51" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="K13" s="51" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="M13" s="14"/>
       <c r="N13" s="25" t="str">
@@ -3381,10 +3381,10 @@
       </c>
       <c r="O13" s="29"/>
       <c r="P13" s="27" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="Q13" s="28" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="S13" s="14"/>
       <c r="T13" s="25" t="str">
@@ -3456,10 +3456,10 @@
       </c>
       <c r="O14" s="29"/>
       <c r="P14" s="27" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="Q14" s="28" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="S14" s="15"/>
       <c r="T14" s="25" t="str">
@@ -3528,10 +3528,10 @@
       </c>
       <c r="O15" s="26"/>
       <c r="P15" s="27" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="Q15" s="28" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="S15" s="15"/>
       <c r="T15" s="25" t="str">
@@ -3604,10 +3604,10 @@
         <v>5</v>
       </c>
       <c r="P16" s="23" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="Q16" s="24" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="S16" s="15"/>
       <c r="T16" s="19" t="str">
@@ -3739,10 +3739,10 @@
         <v>5</v>
       </c>
       <c r="J18" s="52" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="K18" s="52" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="M18" s="15"/>
       <c r="N18" s="25" t="str">
@@ -3751,10 +3751,10 @@
       </c>
       <c r="O18" s="26"/>
       <c r="P18" s="27" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="Q18" s="28" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="S18" s="15"/>
       <c r="T18" s="19" t="str">
@@ -3831,10 +3831,10 @@
         <v>5</v>
       </c>
       <c r="P19" s="23" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="Q19" s="24" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="R19" s="3"/>
       <c r="S19" s="15"/>
@@ -3912,10 +3912,10 @@
       </c>
       <c r="O20" s="26"/>
       <c r="P20" s="27" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="Q20" s="28" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="S20" s="15"/>
       <c r="T20" s="25" t="str">
@@ -3982,10 +3982,10 @@
       </c>
       <c r="O21" s="26"/>
       <c r="P21" s="27" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="Q21" s="28" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="S21" s="15"/>
       <c r="T21" s="25" t="str">
@@ -4054,10 +4054,10 @@
       </c>
       <c r="O22" s="26"/>
       <c r="P22" s="27" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="Q22" s="28" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="S22" s="15"/>
       <c r="T22" s="25" t="str">
@@ -4124,10 +4124,10 @@
       </c>
       <c r="O23" s="26"/>
       <c r="P23" s="27" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q23" s="28" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="S23" s="15"/>
       <c r="T23" s="25" t="str">
@@ -4186,10 +4186,10 @@
       </c>
       <c r="I24" s="29"/>
       <c r="J24" s="51" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="K24" s="51" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="M24" s="14"/>
       <c r="N24" s="25" t="str">
@@ -4198,10 +4198,10 @@
       </c>
       <c r="O24" s="29"/>
       <c r="P24" s="27" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="Q24" s="28" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="S24" s="14"/>
       <c r="T24" s="25" t="str">
@@ -4263,10 +4263,10 @@
       </c>
       <c r="I25" s="29"/>
       <c r="J25" s="51" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="K25" s="51" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="M25" s="15"/>
       <c r="N25" s="25" t="str">
@@ -4275,10 +4275,10 @@
       </c>
       <c r="O25" s="29"/>
       <c r="P25" s="27" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="Q25" s="28" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="S25" s="15"/>
       <c r="T25" s="25" t="str">
@@ -4347,10 +4347,10 @@
       </c>
       <c r="O26" s="26"/>
       <c r="P26" s="27" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="Q26" s="28" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="S26" s="15"/>
       <c r="T26" s="25" t="str">
@@ -4417,10 +4417,10 @@
       </c>
       <c r="O27" s="29"/>
       <c r="P27" s="27" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="Q27" s="28" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="S27" s="15"/>
       <c r="T27" s="25" t="str">
@@ -4560,10 +4560,10 @@
       </c>
       <c r="O29" s="29"/>
       <c r="P29" s="27" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q29" s="28" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="S29" s="15"/>
       <c r="T29" s="25" t="str">
@@ -4630,10 +4630,10 @@
       </c>
       <c r="O30" s="29"/>
       <c r="P30" s="27" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="Q30" s="28" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="S30" s="15"/>
       <c r="T30" s="25" t="str">
@@ -4710,10 +4710,10 @@
         <v>5</v>
       </c>
       <c r="P31" s="23" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="Q31" s="24" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="S31" s="15"/>
       <c r="T31" s="19" t="str">
@@ -4774,10 +4774,10 @@
         <v>5</v>
       </c>
       <c r="J32" s="52" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="K32" s="52" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="M32" s="15"/>
       <c r="N32" s="25" t="str">
@@ -4786,10 +4786,10 @@
       </c>
       <c r="O32" s="26"/>
       <c r="P32" s="27" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="Q32" s="28" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="S32" s="15"/>
       <c r="T32" s="19" t="str">
@@ -4834,10 +4834,10 @@
       </c>
       <c r="C33" s="29"/>
       <c r="D33" s="27" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="G33" s="15"/>
       <c r="H33" s="25" t="str">
@@ -4846,10 +4846,10 @@
       </c>
       <c r="I33" s="29"/>
       <c r="J33" s="51" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="K33" s="51" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="M33" s="15"/>
       <c r="N33" s="25" t="str">
@@ -4858,10 +4858,10 @@
       </c>
       <c r="O33" s="29"/>
       <c r="P33" s="27" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="Q33" s="28" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="S33" s="15"/>
       <c r="T33" s="25" t="str">
@@ -4906,10 +4906,10 @@
       </c>
       <c r="C34" s="29"/>
       <c r="D34" s="27" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="G34" s="15"/>
       <c r="H34" s="25" t="str">
@@ -4918,10 +4918,10 @@
       </c>
       <c r="I34" s="29"/>
       <c r="J34" s="51" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K34" s="51" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="M34" s="15"/>
       <c r="N34" s="25" t="str">
@@ -4930,10 +4930,10 @@
       </c>
       <c r="O34" s="29"/>
       <c r="P34" s="27" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="Q34" s="28" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="S34" s="15"/>
       <c r="T34" s="25" t="str">
@@ -4992,10 +4992,10 @@
       </c>
       <c r="I35" s="29"/>
       <c r="J35" s="51" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="K35" s="51" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="M35" s="14"/>
       <c r="N35" s="25" t="str">
@@ -5004,10 +5004,10 @@
       </c>
       <c r="O35" s="29"/>
       <c r="P35" s="27" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="Q35" s="28" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="S35" s="14"/>
       <c r="T35" s="25" t="str">
@@ -5079,10 +5079,10 @@
       </c>
       <c r="O36" s="29"/>
       <c r="P36" s="27" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="Q36" s="28" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="S36" s="15"/>
       <c r="T36" s="25" t="str">
@@ -5151,10 +5151,10 @@
       </c>
       <c r="O37" s="26"/>
       <c r="P37" s="27" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="Q37" s="28" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="S37" s="15"/>
       <c r="T37" s="25" t="str">
@@ -5227,10 +5227,10 @@
         <v>5</v>
       </c>
       <c r="P38" s="23" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="Q38" s="24" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="S38" s="15"/>
       <c r="T38" s="19" t="str">
@@ -5372,10 +5372,10 @@
       </c>
       <c r="O40" s="29"/>
       <c r="P40" s="27" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="Q40" s="28" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="R40" s="3"/>
       <c r="S40" s="15"/>
@@ -5447,10 +5447,10 @@
       </c>
       <c r="O41" s="29"/>
       <c r="P41" s="27" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="Q41" s="28" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="R41" s="3"/>
       <c r="S41" s="15"/>
@@ -5513,10 +5513,10 @@
         <v>5</v>
       </c>
       <c r="J42" s="52" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="K42" s="52" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="L42" s="3"/>
       <c r="M42" s="15"/>
@@ -5526,10 +5526,10 @@
       </c>
       <c r="O42" s="26"/>
       <c r="P42" s="27" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="Q42" s="28" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="R42" s="3"/>
       <c r="S42" s="15"/>
@@ -5607,10 +5607,10 @@
         <v>5</v>
       </c>
       <c r="P43" s="23" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="Q43" s="24" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="R43" s="3"/>
       <c r="S43" s="15"/>
@@ -5664,25 +5664,23 @@
       </c>
       <c r="C44" s="29"/>
       <c r="D44" s="27" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="E44" s="28" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="F44" s="3"/>
-      <c r="G44" s="15" t="s">
-        <v>5</v>
-      </c>
+      <c r="G44" s="15"/>
       <c r="H44" s="25" t="str">
         <f t="shared" si="18"/>
         <v>NumObj</v>
       </c>
       <c r="I44" s="29"/>
       <c r="J44" s="51" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="K44" s="51" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="L44" s="3"/>
       <c r="M44" s="15"/>
@@ -5692,10 +5690,10 @@
       </c>
       <c r="O44" s="29"/>
       <c r="P44" s="27" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="Q44" s="28" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="R44" s="3"/>
       <c r="S44" s="15"/>
@@ -5756,10 +5754,10 @@
       </c>
       <c r="I45" s="29"/>
       <c r="J45" s="51" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K45" s="51" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="L45" s="3"/>
       <c r="M45" s="15"/>
@@ -5769,10 +5767,10 @@
       </c>
       <c r="O45" s="29"/>
       <c r="P45" s="27" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="Q45" s="28" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="R45" s="3"/>
       <c r="S45" s="15"/>
@@ -5841,10 +5839,10 @@
       </c>
       <c r="I46" s="29"/>
       <c r="J46" s="51" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="K46" s="51" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="L46" s="3"/>
       <c r="M46" s="14"/>
@@ -5854,10 +5852,10 @@
       </c>
       <c r="O46" s="29"/>
       <c r="P46" s="27" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="Q46" s="28" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="R46" s="3"/>
       <c r="S46" s="14"/>
@@ -5918,10 +5916,10 @@
       </c>
       <c r="I47" s="29"/>
       <c r="J47" s="51" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K47" s="51" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="L47" s="3"/>
       <c r="M47" s="15"/>
@@ -5931,10 +5929,10 @@
       </c>
       <c r="O47" s="29"/>
       <c r="P47" s="27" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="Q47" s="28" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="R47" s="3"/>
       <c r="S47" s="15"/>
@@ -6006,10 +6004,10 @@
       </c>
       <c r="O48" s="31"/>
       <c r="P48" s="27" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="Q48" s="28" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="R48" s="3"/>
       <c r="S48" s="15"/>
@@ -6081,10 +6079,10 @@
       </c>
       <c r="O49" s="29"/>
       <c r="P49" s="27" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="Q49" s="28" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="R49" s="3"/>
       <c r="S49" s="15"/>
@@ -6225,10 +6223,10 @@
       </c>
       <c r="O51" s="29"/>
       <c r="P51" s="27" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="Q51" s="28" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="S51" s="15"/>
       <c r="T51" s="25" t="str">
@@ -6295,10 +6293,10 @@
       </c>
       <c r="O52" s="29"/>
       <c r="P52" s="27" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="Q52" s="28" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="S52" s="15"/>
       <c r="T52" s="25" t="str">
@@ -6345,10 +6343,10 @@
       </c>
       <c r="C53" s="29"/>
       <c r="D53" s="27" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="G53" s="15"/>
       <c r="H53" s="25" t="str">
@@ -6357,10 +6355,10 @@
       </c>
       <c r="I53" s="26"/>
       <c r="J53" s="51" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="K53" s="51" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="M53" s="15"/>
       <c r="N53" s="25" t="str">
@@ -6369,10 +6367,10 @@
       </c>
       <c r="O53" s="26"/>
       <c r="P53" s="27" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="Q53" s="28" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="S53" s="15"/>
       <c r="T53" s="19" t="str">
@@ -6415,10 +6413,10 @@
       </c>
       <c r="C54" s="29"/>
       <c r="D54" s="27" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E54" s="28" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="G54" s="15"/>
       <c r="H54" s="25" t="str">
@@ -6427,10 +6425,10 @@
       </c>
       <c r="I54" s="26"/>
       <c r="J54" s="51" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="K54" s="51" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="M54" s="15"/>
       <c r="N54" s="25" t="str">
@@ -6439,10 +6437,10 @@
       </c>
       <c r="O54" s="26"/>
       <c r="P54" s="27" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="Q54" s="28" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="S54" s="15"/>
       <c r="T54" s="19" t="str">
@@ -6517,10 +6515,10 @@
         <v>5</v>
       </c>
       <c r="P55" s="23" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="Q55" s="24" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="S55" s="15"/>
       <c r="T55" s="19" t="str">
@@ -6581,10 +6579,10 @@
         <v>5</v>
       </c>
       <c r="J56" s="52" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="K56" s="52" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="M56" s="15"/>
       <c r="N56" s="25" t="str">
@@ -6593,10 +6591,10 @@
       </c>
       <c r="O56" s="26"/>
       <c r="P56" s="27" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="Q56" s="28" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="S56" s="15"/>
       <c r="T56" s="19" t="str">
@@ -6655,10 +6653,10 @@
       </c>
       <c r="I57" s="29"/>
       <c r="J57" s="51" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="K57" s="51" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="M57" s="14"/>
       <c r="N57" s="25" t="str">
@@ -6667,10 +6665,10 @@
       </c>
       <c r="O57" s="29"/>
       <c r="P57" s="27" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="Q57" s="28" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="S57" s="14"/>
       <c r="T57" s="25" t="str">
@@ -6730,10 +6728,10 @@
       </c>
       <c r="I58" s="29"/>
       <c r="J58" s="51" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="K58" s="51" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="M58" s="15"/>
       <c r="N58" s="25" t="str">
@@ -6742,10 +6740,10 @@
       </c>
       <c r="O58" s="29"/>
       <c r="P58" s="27" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="Q58" s="28" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="S58" s="15"/>
       <c r="T58" s="25" t="str">
@@ -6814,10 +6812,10 @@
       </c>
       <c r="O59" s="26"/>
       <c r="P59" s="27" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="Q59" s="28" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="S59" s="15"/>
       <c r="T59" s="25" t="str">
@@ -6890,10 +6888,10 @@
         <v>5</v>
       </c>
       <c r="P60" s="23" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="Q60" s="24" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="S60" s="15"/>
       <c r="T60" s="19" t="str">
@@ -7033,10 +7031,10 @@
       </c>
       <c r="O62" s="29"/>
       <c r="P62" s="27" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="Q62" s="28" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="S62" s="15"/>
       <c r="T62" s="25" t="str">
@@ -7103,10 +7101,10 @@
       </c>
       <c r="O63" s="29"/>
       <c r="P63" s="27" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="Q63" s="28" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="S63" s="15"/>
       <c r="T63" s="25" t="str">
@@ -7153,10 +7151,10 @@
       </c>
       <c r="C64" s="26"/>
       <c r="D64" s="27" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="E64" s="28" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G64" s="15"/>
       <c r="H64" s="25" t="str">
@@ -7165,10 +7163,10 @@
       </c>
       <c r="I64" s="26"/>
       <c r="J64" s="51" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="K64" s="51" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="M64" s="15"/>
       <c r="N64" s="25" t="str">
@@ -7177,10 +7175,10 @@
       </c>
       <c r="O64" s="26"/>
       <c r="P64" s="27" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="Q64" s="28" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="S64" s="15"/>
       <c r="T64" s="19" t="str">
@@ -7253,10 +7251,10 @@
         <v>5</v>
       </c>
       <c r="P65" s="23" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="Q65" s="24" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="S65" s="15"/>
       <c r="T65" s="19" t="str">
@@ -7335,10 +7333,10 @@
         <v>5</v>
       </c>
       <c r="J66" s="52" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="K66" s="52" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="M66" s="15"/>
       <c r="N66" s="25" t="str">
@@ -7347,10 +7345,10 @@
       </c>
       <c r="O66" s="26"/>
       <c r="P66" s="27" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="Q66" s="28" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="S66" s="15"/>
       <c r="T66" s="19" t="str">
@@ -7425,10 +7423,10 @@
         <v>5</v>
       </c>
       <c r="P67" s="23" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="Q67" s="24" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="S67" s="15"/>
       <c r="T67" s="19" t="str">
@@ -7505,10 +7503,10 @@
       </c>
       <c r="I68" s="29"/>
       <c r="J68" s="51" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="K68" s="51" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="M68" s="14"/>
       <c r="N68" s="25" t="str">
@@ -7517,10 +7515,10 @@
       </c>
       <c r="O68" s="29"/>
       <c r="P68" s="27" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="Q68" s="28" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="S68" s="14"/>
       <c r="T68" s="25" t="str">
@@ -7582,10 +7580,10 @@
       </c>
       <c r="I69" s="29"/>
       <c r="J69" s="51" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="K69" s="51" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="M69" s="15"/>
       <c r="N69" s="25" t="str">
@@ -7594,10 +7592,10 @@
       </c>
       <c r="O69" s="29"/>
       <c r="P69" s="27" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="Q69" s="28" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="S69" s="15"/>
       <c r="T69" s="25" t="str">
@@ -7654,10 +7652,10 @@
       </c>
       <c r="I70" s="26"/>
       <c r="J70" s="51" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K70" s="51" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="M70" s="15"/>
       <c r="N70" s="25" t="str">
@@ -7666,10 +7664,10 @@
       </c>
       <c r="O70" s="26"/>
       <c r="P70" s="27" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="Q70" s="28" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="S70" s="15"/>
       <c r="T70" s="25" t="str">
@@ -7724,10 +7722,10 @@
       </c>
       <c r="I71" s="29"/>
       <c r="J71" s="51" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="K71" s="51" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="M71" s="15"/>
       <c r="N71" s="25" t="str">
@@ -7736,10 +7734,10 @@
       </c>
       <c r="O71" s="29"/>
       <c r="P71" s="27" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="Q71" s="28" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="S71" s="15"/>
       <c r="T71" s="25" t="str">
@@ -7885,10 +7883,10 @@
         <v>5</v>
       </c>
       <c r="P73" s="23" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="Q73" s="24" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="S73" s="15"/>
       <c r="T73" s="19" t="str">
@@ -7947,10 +7945,10 @@
         <v>5</v>
       </c>
       <c r="J74" s="52" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="K74" s="52" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="M74" s="15"/>
       <c r="N74" s="25" t="str">
@@ -7959,10 +7957,10 @@
       </c>
       <c r="O74" s="29"/>
       <c r="P74" s="27" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="Q74" s="28" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="S74" s="15"/>
       <c r="T74" s="25" t="str">
@@ -8039,10 +8037,10 @@
         <v>5</v>
       </c>
       <c r="P75" s="23" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="Q75" s="24" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="S75" s="15"/>
       <c r="T75" s="19" t="str">
@@ -8101,10 +8099,10 @@
         <v>5</v>
       </c>
       <c r="J76" s="52" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="K76" s="52" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="M76" s="15"/>
       <c r="N76" s="25" t="str">
@@ -8113,10 +8111,10 @@
       </c>
       <c r="O76" s="29"/>
       <c r="P76" s="27" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="Q76" s="28" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="S76" s="15"/>
       <c r="T76" s="25" t="str">
@@ -8191,10 +8189,10 @@
         <v>5</v>
       </c>
       <c r="P77" s="23" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="Q77" s="24" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S77" s="15"/>
       <c r="T77" s="19" t="str">
@@ -8253,10 +8251,10 @@
         <v>5</v>
       </c>
       <c r="J78" s="52" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="K78" s="52" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="M78" s="15"/>
       <c r="N78" s="25" t="str">
@@ -8265,10 +8263,10 @@
       </c>
       <c r="O78" s="29"/>
       <c r="P78" s="27" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="Q78" s="28" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="S78" s="15"/>
       <c r="T78" s="25" t="str">
@@ -8343,10 +8341,10 @@
         <v>5</v>
       </c>
       <c r="P79" s="23" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="Q79" s="24" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="S79" s="14"/>
       <c r="T79" s="19" t="str">
@@ -8407,10 +8405,10 @@
         <v>5</v>
       </c>
       <c r="J80" s="52" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="K80" s="52" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="M80" s="15"/>
       <c r="N80" s="25" t="str">
@@ -8419,10 +8417,10 @@
       </c>
       <c r="O80" s="29"/>
       <c r="P80" s="27" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="Q80" s="28" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="S80" s="15"/>
       <c r="T80" s="25" t="str">
@@ -8515,10 +8513,10 @@
         <v>5</v>
       </c>
       <c r="P81" s="23" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="Q81" s="24" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="S81" s="15"/>
       <c r="T81" s="19" t="str">
@@ -8593,10 +8591,10 @@
         <v>5</v>
       </c>
       <c r="P82" s="23" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="Q82" s="24" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="S82" s="15"/>
       <c r="T82" s="19" t="str">
@@ -8754,10 +8752,10 @@
       </c>
       <c r="O84" s="29"/>
       <c r="P84" s="27" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="Q84" s="28" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="S84" s="15"/>
       <c r="T84" s="25" t="str">
@@ -8814,10 +8812,10 @@
       </c>
       <c r="I85" s="29"/>
       <c r="J85" s="51" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="K85" s="51" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="M85" s="15"/>
       <c r="N85" s="25" t="str">
@@ -8826,10 +8824,10 @@
       </c>
       <c r="O85" s="29"/>
       <c r="P85" s="27" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="Q85" s="28" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="S85" s="15"/>
       <c r="T85" s="25" t="str">
@@ -8888,10 +8886,10 @@
       </c>
       <c r="I86" s="29"/>
       <c r="J86" s="51" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="K86" s="51" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="M86" s="15"/>
       <c r="N86" s="25" t="str">
@@ -8900,10 +8898,10 @@
       </c>
       <c r="O86" s="29"/>
       <c r="P86" s="27" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="Q86" s="28" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="S86" s="15"/>
       <c r="T86" s="25" t="str">
@@ -8960,10 +8958,10 @@
       </c>
       <c r="I87" s="29"/>
       <c r="J87" s="51" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="K87" s="51" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="M87" s="15"/>
       <c r="N87" s="25" t="str">
@@ -8972,10 +8970,10 @@
       </c>
       <c r="O87" s="29"/>
       <c r="P87" s="27" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="Q87" s="28" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="S87" s="15"/>
       <c r="T87" s="25" t="str">
@@ -9032,10 +9030,10 @@
       </c>
       <c r="I88" s="26"/>
       <c r="J88" s="51" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="K88" s="51" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="M88" s="15"/>
       <c r="N88" s="25" t="str">
@@ -9044,10 +9042,10 @@
       </c>
       <c r="O88" s="26"/>
       <c r="P88" s="27" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="Q88" s="28" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="S88" s="15"/>
       <c r="T88" s="25" t="str">
@@ -9104,10 +9102,10 @@
       </c>
       <c r="I89" s="29"/>
       <c r="J89" s="51" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="K89" s="51" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="M89" s="15"/>
       <c r="N89" s="25" t="str">
@@ -9116,10 +9114,10 @@
       </c>
       <c r="O89" s="29"/>
       <c r="P89" s="27" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="Q89" s="28" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="S89" s="15"/>
       <c r="T89" s="25" t="str">
@@ -9178,10 +9176,10 @@
       </c>
       <c r="I90" s="29"/>
       <c r="J90" s="51" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="K90" s="51" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="M90" s="14"/>
       <c r="N90" s="25" t="str">
@@ -9190,10 +9188,10 @@
       </c>
       <c r="O90" s="29"/>
       <c r="P90" s="27" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="Q90" s="28" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="S90" s="14"/>
       <c r="T90" s="25" t="str">
@@ -9268,10 +9266,10 @@
         <v>5</v>
       </c>
       <c r="P91" s="23" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="Q91" s="24" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="S91" s="15"/>
       <c r="T91" s="19" t="str">
@@ -9350,10 +9348,10 @@
         <v>5</v>
       </c>
       <c r="J92" s="52" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="K92" s="52" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="M92" s="15"/>
       <c r="N92" s="25" t="str">
@@ -9362,10 +9360,10 @@
       </c>
       <c r="O92" s="26"/>
       <c r="P92" s="27" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="Q92" s="28" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="S92" s="15"/>
       <c r="T92" s="19" t="str">
@@ -9418,18 +9416,16 @@
         <v>179</v>
       </c>
       <c r="G93" s="15"/>
-      <c r="H93" s="19" t="str">
+      <c r="H93" s="25" t="str">
         <f t="shared" si="42"/>
         <v>undefined</v>
       </c>
-      <c r="I93" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="J93" s="52" t="s">
-        <v>344</v>
-      </c>
-      <c r="K93" s="52" t="s">
-        <v>345</v>
+      <c r="I93" s="29"/>
+      <c r="J93" s="51" t="s">
+        <v>638</v>
+      </c>
+      <c r="K93" s="51" t="s">
+        <v>639</v>
       </c>
       <c r="M93" s="15"/>
       <c r="N93" s="19" t="str">
@@ -9440,10 +9436,10 @@
         <v>5</v>
       </c>
       <c r="P93" s="23" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="Q93" s="24" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="S93" s="15"/>
       <c r="T93" s="19" t="str">
@@ -9589,10 +9585,10 @@
       </c>
       <c r="I95" s="26"/>
       <c r="J95" s="51" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K95" s="51" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="M95" s="15"/>
       <c r="N95" s="25" t="str">
@@ -9601,10 +9597,10 @@
       </c>
       <c r="O95" s="26"/>
       <c r="P95" s="27" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="Q95" s="28" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="S95" s="15"/>
       <c r="T95" s="25" t="str">
@@ -9659,10 +9655,10 @@
       </c>
       <c r="I96" s="26"/>
       <c r="J96" s="51" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="K96" s="51" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="M96" s="15"/>
       <c r="N96" s="25" t="str">
@@ -9671,10 +9667,10 @@
       </c>
       <c r="O96" s="26"/>
       <c r="P96" s="27" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="Q96" s="28" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="S96" s="15"/>
       <c r="T96" s="25" t="str">
@@ -9733,10 +9729,10 @@
       </c>
       <c r="I97" s="26"/>
       <c r="J97" s="51" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="K97" s="51" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="M97" s="15"/>
       <c r="N97" s="25" t="str">
@@ -9745,10 +9741,10 @@
       </c>
       <c r="O97" s="26"/>
       <c r="P97" s="27" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="Q97" s="28" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="S97" s="15"/>
       <c r="T97" s="25" t="str">
@@ -9803,10 +9799,10 @@
       </c>
       <c r="I98" s="26"/>
       <c r="J98" s="51" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="K98" s="51" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="M98" s="15"/>
       <c r="N98" s="25" t="str">
@@ -9815,10 +9811,10 @@
       </c>
       <c r="O98" s="26"/>
       <c r="P98" s="27" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="Q98" s="28" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="S98" s="15"/>
       <c r="T98" s="25" t="str">
@@ -9875,10 +9871,10 @@
       </c>
       <c r="I99" s="26"/>
       <c r="J99" s="51" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K99" s="51" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="M99" s="15"/>
       <c r="N99" s="25" t="str">
@@ -9887,10 +9883,10 @@
       </c>
       <c r="O99" s="26"/>
       <c r="P99" s="27" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="Q99" s="28" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="S99" s="15"/>
       <c r="T99" s="25" t="str">
@@ -9945,10 +9941,10 @@
       </c>
       <c r="I100" s="26"/>
       <c r="J100" s="51" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="K100" s="51" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="M100" s="15"/>
       <c r="N100" s="25" t="str">
@@ -9957,10 +9953,10 @@
       </c>
       <c r="O100" s="26"/>
       <c r="P100" s="27" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="Q100" s="28" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="S100" s="15"/>
       <c r="T100" s="25" t="str">
@@ -10021,10 +10017,10 @@
       </c>
       <c r="I101" s="26"/>
       <c r="J101" s="51" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="K101" s="51" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="M101" s="14"/>
       <c r="N101" s="25" t="str">
@@ -10033,10 +10029,10 @@
       </c>
       <c r="O101" s="29"/>
       <c r="P101" s="27" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="Q101" s="28" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="S101" s="14"/>
       <c r="T101" s="25" t="str">
@@ -10097,10 +10093,10 @@
         <v>5</v>
       </c>
       <c r="J102" s="52" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="K102" s="52" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="M102" s="15"/>
       <c r="N102" s="25" t="str">
@@ -10109,10 +10105,10 @@
       </c>
       <c r="O102" s="26"/>
       <c r="P102" s="27" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="Q102" s="28" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="S102" s="15"/>
       <c r="T102" s="19" t="str">
@@ -10173,10 +10169,10 @@
         <v>77</v>
       </c>
       <c r="J103" s="52" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="K103" s="52" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="M103" s="15"/>
       <c r="N103" s="19" t="str">
@@ -10187,10 +10183,10 @@
         <v>5</v>
       </c>
       <c r="P103" s="23" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="Q103" s="24" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="S103" s="15"/>
       <c r="T103" s="19" t="str">
@@ -10251,10 +10247,10 @@
         <v>5</v>
       </c>
       <c r="J104" s="52" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="K104" s="52" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="M104" s="15"/>
       <c r="N104" s="19" t="str">
@@ -10265,10 +10261,10 @@
         <v>5</v>
       </c>
       <c r="P104" s="23" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="Q104" s="24" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="S104" s="15"/>
       <c r="T104" s="19" t="str">
@@ -10396,10 +10392,10 @@
       </c>
       <c r="I106" s="33"/>
       <c r="J106" s="51" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="K106" s="51" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="M106" s="18"/>
       <c r="N106" s="32" t="str">
@@ -10408,10 +10404,10 @@
       </c>
       <c r="O106" s="33"/>
       <c r="P106" s="34" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="Q106" s="35" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="S106" s="18"/>
       <c r="T106" s="32" t="str">
@@ -11032,44 +11028,44 @@
     <hyperlink ref="K91" r:id="rId506"/>
     <hyperlink ref="J92" r:id="rId507"/>
     <hyperlink ref="K92" r:id="rId508"/>
-    <hyperlink ref="J93" r:id="rId509"/>
-    <hyperlink ref="K93" r:id="rId510"/>
-    <hyperlink ref="J95" r:id="rId511"/>
-    <hyperlink ref="K95" r:id="rId512"/>
-    <hyperlink ref="J96" r:id="rId513"/>
-    <hyperlink ref="K96" r:id="rId514"/>
-    <hyperlink ref="J97" r:id="rId515"/>
-    <hyperlink ref="K97" r:id="rId516"/>
-    <hyperlink ref="J98" r:id="rId517"/>
-    <hyperlink ref="K98" r:id="rId518"/>
-    <hyperlink ref="J99" r:id="rId519"/>
-    <hyperlink ref="K99" r:id="rId520"/>
-    <hyperlink ref="J100" r:id="rId521"/>
-    <hyperlink ref="K100" r:id="rId522"/>
-    <hyperlink ref="J101" r:id="rId523" display="Pass\ImpAssignTextObjObject.quorum"/>
-    <hyperlink ref="K101" r:id="rId524" display="Pass\ImpAssignTextObjObjectField.quorum"/>
-    <hyperlink ref="J103" r:id="rId525"/>
-    <hyperlink ref="K103" r:id="rId526"/>
-    <hyperlink ref="J104" r:id="rId527"/>
-    <hyperlink ref="K104" r:id="rId528"/>
-    <hyperlink ref="J106" r:id="rId529"/>
-    <hyperlink ref="K106" r:id="rId530"/>
-    <hyperlink ref="J8" r:id="rId531"/>
-    <hyperlink ref="K8" r:id="rId532"/>
-    <hyperlink ref="J32" r:id="rId533"/>
-    <hyperlink ref="K32" r:id="rId534"/>
-    <hyperlink ref="J56" r:id="rId535"/>
-    <hyperlink ref="K56" r:id="rId536"/>
-    <hyperlink ref="J74" r:id="rId537"/>
-    <hyperlink ref="K74" r:id="rId538"/>
-    <hyperlink ref="K76" r:id="rId539"/>
-    <hyperlink ref="J76" r:id="rId540"/>
-    <hyperlink ref="J78" r:id="rId541"/>
-    <hyperlink ref="K78" r:id="rId542"/>
-    <hyperlink ref="K80" r:id="rId543"/>
-    <hyperlink ref="J80" r:id="rId544"/>
-    <hyperlink ref="J102" r:id="rId545"/>
-    <hyperlink ref="K102" r:id="rId546"/>
+    <hyperlink ref="K93" r:id="rId509"/>
+    <hyperlink ref="J95" r:id="rId510"/>
+    <hyperlink ref="K95" r:id="rId511"/>
+    <hyperlink ref="J96" r:id="rId512"/>
+    <hyperlink ref="K96" r:id="rId513"/>
+    <hyperlink ref="J97" r:id="rId514"/>
+    <hyperlink ref="K97" r:id="rId515"/>
+    <hyperlink ref="J98" r:id="rId516"/>
+    <hyperlink ref="K98" r:id="rId517"/>
+    <hyperlink ref="J99" r:id="rId518"/>
+    <hyperlink ref="K99" r:id="rId519"/>
+    <hyperlink ref="J100" r:id="rId520"/>
+    <hyperlink ref="K100" r:id="rId521"/>
+    <hyperlink ref="J101" r:id="rId522" display="Pass\ImpAssignTextObjObject.quorum"/>
+    <hyperlink ref="K101" r:id="rId523" display="Pass\ImpAssignTextObjObjectField.quorum"/>
+    <hyperlink ref="J103" r:id="rId524"/>
+    <hyperlink ref="K103" r:id="rId525"/>
+    <hyperlink ref="J104" r:id="rId526"/>
+    <hyperlink ref="K104" r:id="rId527"/>
+    <hyperlink ref="J106" r:id="rId528"/>
+    <hyperlink ref="K106" r:id="rId529"/>
+    <hyperlink ref="J8" r:id="rId530"/>
+    <hyperlink ref="K8" r:id="rId531"/>
+    <hyperlink ref="J32" r:id="rId532"/>
+    <hyperlink ref="K32" r:id="rId533"/>
+    <hyperlink ref="J56" r:id="rId534"/>
+    <hyperlink ref="K56" r:id="rId535"/>
+    <hyperlink ref="J74" r:id="rId536"/>
+    <hyperlink ref="K74" r:id="rId537"/>
+    <hyperlink ref="K76" r:id="rId538"/>
+    <hyperlink ref="J76" r:id="rId539"/>
+    <hyperlink ref="J78" r:id="rId540"/>
+    <hyperlink ref="K78" r:id="rId541"/>
+    <hyperlink ref="K80" r:id="rId542"/>
+    <hyperlink ref="J80" r:id="rId543"/>
+    <hyperlink ref="J102" r:id="rId544"/>
+    <hyperlink ref="K102" r:id="rId545"/>
+    <hyperlink ref="J93" r:id="rId546"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId547"/>
@@ -11094,42 +11090,42 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -11153,7 +11149,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N93"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
       <selection activeCell="I3" sqref="I3:I93"/>
     </sheetView>
   </sheetViews>
@@ -15155,11 +15151,11 @@
       </c>
       <c r="H82" t="str">
         <f>IF('Quorum 3.0'!I93="x", "Pass", "Fail")</f>
-        <v>Pass</v>
+        <v>Fail</v>
       </c>
       <c r="I82" t="str">
         <f t="shared" si="4"/>
-        <v>text,undefined,Pass</v>
+        <v>text,undefined,Fail</v>
       </c>
       <c r="K82" t="str">
         <f>'Quorum 3.0'!M$83</f>

</xml_diff>